<commit_message>
4 data set filled and working...
</commit_message>
<xml_diff>
--- a/Casos de prueba/Casos de prueba TFI.xlsx
+++ b/Casos de prueba/Casos de prueba TFI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hernan\Desktop\Development\TFI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haria\Repositories\TFI-BackEnd\Casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6726554E-B5E5-48AC-B9A7-FD40428CD23C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0106CF44-C1CF-407C-9994-6F7FA19D1F00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{E19D2194-C2B1-4B6D-9336-FDF693023F08}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" firstSheet="3" activeTab="8" xr2:uid="{E19D2194-C2B1-4B6D-9336-FDF693023F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="Caso 4(ETAs) (Canc 0.2)" sheetId="8" r:id="rId7"/>
     <sheet name="Caso 5(ETAs) (Adelantar)" sheetId="9" r:id="rId8"/>
     <sheet name="Pacientes" sheetId="11" r:id="rId9"/>
-    <sheet name="CodeLineRunner" sheetId="12" r:id="rId10"/>
+    <sheet name="Usuarios" sheetId="13" r:id="rId10"/>
+    <sheet name="CodeLineRunner" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2672" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="309">
   <si>
     <t>Operacion</t>
   </si>
@@ -840,9 +841,6 @@
     <t>tempPatient = new Patient("Julio", "Arias", LocalDate.of(1953, 1, 17), 10664879, 1, "Lanus", false, true, false, false, false); patientRepository.save(tempPatient);</t>
   </si>
   <si>
-    <t>tempPatient = new Patient("Beatriz", "Leguizamon", LocalDate.of(1955, 6, 25), 9215788, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</t>
-  </si>
-  <si>
     <t>tempPatient = new Patient("Cristian", "Vallarino", LocalDate.of(1983, 2, 22), 30127532, 1, "Banfield", true, false, false, false, false); patientRepository.save(tempPatient);</t>
   </si>
   <si>
@@ -958,6 +956,51 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>tempPatient = new Patient("Beatriz"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Leguizamon"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LocalDate.of(1955</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Lanus"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> true</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> false</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> false); patientRepository.save(tempPatient);</t>
+  </si>
+  <si>
+    <t>tempPatient = new Patient("Julio"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Arias"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LocalDate.of(1953</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17)</t>
   </si>
 </sst>
 </file>
@@ -1378,11 +1421,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="12" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="12" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="12" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="5" fillId="12" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1390,19 +1447,16 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1420,20 +1474,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1450,17 +1504,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="12" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="5" fillId="12" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="5" fillId="12" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="5" fillId="12" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
@@ -1783,27 +1826,27 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="31.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="31.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26171875" customWidth="1"/>
+    <col min="3" max="3" width="31.15625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.15625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
@@ -1823,7 +1866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
         <v>210</v>
       </c>
@@ -1839,7 +1882,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
         <v>211</v>
       </c>
@@ -1855,17 +1898,17 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
@@ -1885,7 +1928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>212</v>
       </c>
@@ -1901,7 +1944,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>213</v>
       </c>
@@ -1917,19 +1960,19 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="8" t="s">
         <v>198</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -1949,7 +1992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>206</v>
       </c>
@@ -1965,7 +2008,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
@@ -1985,7 +2028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="7" t="s">
         <v>207</v>
       </c>
@@ -2001,7 +2044,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5" t="s">
         <v>51</v>
       </c>
@@ -2021,7 +2064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7" t="s">
         <v>208</v>
       </c>
@@ -2037,7 +2080,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5" t="s">
         <v>51</v>
       </c>
@@ -2057,7 +2100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="7" t="s">
         <v>209</v>
       </c>
@@ -2073,19 +2116,19 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="8" t="s">
         <v>199</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -2105,7 +2148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="7" t="s">
         <v>200</v>
       </c>
@@ -2121,7 +2164,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5" t="s">
         <v>51</v>
       </c>
@@ -2141,7 +2184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7" t="s">
         <v>201</v>
       </c>
@@ -2157,7 +2200,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7" t="s">
         <v>202</v>
       </c>
@@ -2173,7 +2216,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
@@ -2193,7 +2236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
         <v>203</v>
       </c>
@@ -2209,7 +2252,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
         <v>59</v>
       </c>
@@ -2225,7 +2268,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5" t="s">
         <v>51</v>
       </c>
@@ -2245,7 +2288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7" t="s">
         <v>204</v>
       </c>
@@ -2261,7 +2304,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5" t="s">
         <v>51</v>
       </c>
@@ -2281,7 +2324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="7" t="s">
         <v>205</v>
       </c>
@@ -2310,6 +2353,38 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F947F389-137E-47A9-B6AD-45D161DF4B81}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="str">
+        <f>Pacientes!C2</f>
+        <v>"Julio"</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75605B5-9BA1-4DBA-9958-FDD7A98EA7A9}">
   <dimension ref="A1:I37"/>
   <sheetViews>
@@ -2317,34 +2392,34 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="5" width="20.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
-        <v>294</v>
-      </c>
-      <c r="B1" s="75" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="50" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>290</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="D1" s="50" t="s">
         <v>291</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="E1" s="50" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="45" t="s">
         <v>292</v>
       </c>
-      <c r="E1" s="75" t="s">
-        <v>291</v>
-      </c>
-      <c r="I1" s="70" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
-        <f>Pacientes!A1</f>
+        <f>Pacientes!B2</f>
         <v>tempPatient = new Patient("Julio", "Arias", LocalDate.of(1953, 1, 17), 10664879, 1, "Lanus", false, true, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B2" t="str">
@@ -2366,10 +2441,10 @@
         <v>tempPatient = new Patient("Julio", "Arias", LocalDate.of(1953, 1, 17), 10664879, 1, "Lanus", false, true, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(9,0), false, LocalTime.of(9,20),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(9,0), false, LocalTime.of(9,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
-        <f>Pacientes!A2</f>
-        <v>tempPatient = new Patient("Beatriz", "Leguizamon", LocalDate.of(1955, 6, 25), 9215788, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
+        <f>Pacientes!B3</f>
+        <v>tempPatient = new Patient("Beatriz"</v>
       </c>
       <c r="B3" t="str">
         <f>'Caso 1(ETAs)'!K4</f>
@@ -2387,12 +2462,12 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I37" si="0">_xlfn.CONCAT(A3,B3,C3,D3,E3)</f>
-        <v>tempPatient = new Patient("Beatriz", "Leguizamon", LocalDate.of(1955, 6, 25), 9215788, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(9,20), false, LocalTime.of(9,35),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(9,15), false, LocalTime.of(9,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>tempPatient = new Patient("Beatriz"tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(9,20), false, LocalTime.of(9,35),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(9,15), false, LocalTime.of(9,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
-        <f>Pacientes!A3</f>
+        <f>Pacientes!B4</f>
         <v>tempPatient = new Patient("Cristian", "Vallarino", LocalDate.of(1983, 2, 22), 30127532, 1, "Banfield", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B4" t="str">
@@ -2414,9 +2489,9 @@
         <v>tempPatient = new Patient("Cristian", "Vallarino", LocalDate.of(1983, 2, 22), 30127532, 1, "Banfield", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(9,35), false, LocalTime.of(10,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(9,30), false, LocalTime.of(9,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
-        <f>Pacientes!A4</f>
+        <f>Pacientes!B5</f>
         <v>tempPatient = new Patient("Victoria", "Arias", LocalDate.of(1980, 1, 25), 26742442, 2, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B5" t="str">
@@ -2438,9 +2513,9 @@
         <v>tempPatient = new Patient("Victoria", "Arias", LocalDate.of(1980, 1, 25), 26742442, 2, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(10,0), false, LocalTime.of(10,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(9,45), false, LocalTime.of(10,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="str">
-        <f>Pacientes!A5</f>
+        <f>Pacientes!B6</f>
         <v>tempPatient = new Patient("Camila", "Garcia", LocalDate.of(1982, 7, 9), 30333982, 2, "Lomas", false, false, true, false, true); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B6" t="str">
@@ -2462,9 +2537,9 @@
         <v>tempPatient = new Patient("Camila", "Garcia", LocalDate.of(1982, 7, 9), 30333982, 2, "Lomas", false, false, true, false, true); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(10,15), false, LocalTime.of(10,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(10,0), true, LocalTime.of(10,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="str">
-        <f>Pacientes!A6</f>
+        <f>Pacientes!B7</f>
         <v>tempPatient = new Patient("Gabriela", "Suarez", LocalDate.of(1981, 11, 11), 28447445, 2, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B7" t="str">
@@ -2486,9 +2561,9 @@
         <v>tempPatient = new Patient("Gabriela", "Suarez", LocalDate.of(1981, 11, 11), 28447445, 2, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(10,30), false, LocalTime.of(10,50),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(10,15), false, LocalTime.of(10,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
-        <f>Pacientes!A7</f>
+        <f>Pacientes!B8</f>
         <v>tempPatient = new Patient("Francisco", "De Marco", LocalDate.of(1978, 9, 10), 25725839, 1, "CABA", true, true, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B8" t="str">
@@ -2510,9 +2585,9 @@
         <v>tempPatient = new Patient("Francisco", "De Marco", LocalDate.of(1978, 9, 10), 25725839, 1, "CABA", true, true, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(10,50), false, LocalTime.of(11,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(10,30), false, LocalTime.of(10,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
-        <f>Pacientes!A8</f>
+        <f>Pacientes!B9</f>
         <v>tempPatient = new Patient("Emilio", "Dissi", LocalDate.of(1970, 3, 3), 20876091, 1, "Lomas", true, true, true, true, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B9" t="str">
@@ -2534,9 +2609,9 @@
         <v>tempPatient = new Patient("Emilio", "Dissi", LocalDate.of(1970, 3, 3), 20876091, 1, "Lomas", true, true, true, true, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(11,0), false, LocalTime.of(11,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(10,45), false, LocalTime.of(11,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
-        <f>Pacientes!A9</f>
+        <f>Pacientes!B10</f>
         <v>tempPatient = new Patient("Iris", "De Ojo", LocalDate.of(1985, 9, 1), 33445775, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B10" t="str">
@@ -2558,9 +2633,9 @@
         <v>tempPatient = new Patient("Iris", "De Ojo", LocalDate.of(1985, 9, 1), 33445775, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(11,15), false, LocalTime.of(11,35),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(11,0), false, LocalTime.of(11,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
-        <f>Pacientes!A10</f>
+        <f>Pacientes!B11</f>
         <v>tempPatient = new Patient("Luciano", "Lunga", LocalDate.of(1981, 11, 11), 22987456, 1, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B11" t="str">
@@ -2582,9 +2657,9 @@
         <v>tempPatient = new Patient("Luciano", "Lunga", LocalDate.of(1981, 11, 11), 22987456, 1, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(11,35), false, LocalTime.of(11,40),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(11,15), true, LocalTime.of(11,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="str">
-        <f>Pacientes!A11</f>
+        <f>Pacientes!B12</f>
         <v>tempPatient = new Patient("Alejo", "Perez", LocalDate.of(1982, 2, 15), 29851753, 1, "Temperley", false, false, false, true, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B12" t="str">
@@ -2606,9 +2681,9 @@
         <v>tempPatient = new Patient("Alejo", "Perez", LocalDate.of(1982, 2, 15), 29851753, 1, "Temperley", false, false, false, true, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(11,40), false, LocalTime.of(12,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(11,30), false, LocalTime.of(11,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="str">
-        <f>Pacientes!A12</f>
+        <f>Pacientes!B13</f>
         <v>tempPatient = new Patient("Paula", "Perez", LocalDate.of(1980, 2, 25), 29356543, 2, "Lanus", false, true, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B13" t="str">
@@ -2630,9 +2705,9 @@
         <v>tempPatient = new Patient("Paula", "Perez", LocalDate.of(1980, 2, 25), 29356543, 2, "Lanus", false, true, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(12,0), false, LocalTime.of(12,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(11,45), true, LocalTime.of(12,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
-        <f>Pacientes!A13</f>
+        <f>Pacientes!B14</f>
         <v>tempPatient = new Patient("Julio", "Sanchez", LocalDate.of(1955, 5, 15), 12615229, 1, "Lanus", false, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B14" t="str">
@@ -2654,9 +2729,9 @@
         <v>tempPatient = new Patient("Julio", "Sanchez", LocalDate.of(1955, 5, 15), 12615229, 1, "Lanus", false, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(12,15), false, LocalTime.of(12,35),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(12,0), false, LocalTime.of(12,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
-        <f>Pacientes!A14</f>
+        <f>Pacientes!B15</f>
         <v>tempPatient = new Patient("Laura", "Bonilla", LocalDate.of(1984, 5, 15), 33153323, 2, "Lanus", false, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B15" t="str">
@@ -2678,9 +2753,9 @@
         <v>tempPatient = new Patient("Laura", "Bonilla", LocalDate.of(1984, 5, 15), 33153323, 2, "Lanus", false, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(12,35), false, LocalTime.of(12,55),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(12,15), false, LocalTime.of(12,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
-        <f>Pacientes!A15</f>
+        <f>Pacientes!B16</f>
         <v>tempPatient = new Patient("Andrea", "Gonzales", LocalDate.of(1982, 2, 27), 29445256, 2, "Temperlay", true, true, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B16" t="str">
@@ -2702,9 +2777,9 @@
         <v>tempPatient = new Patient("Andrea", "Gonzales", LocalDate.of(1982, 2, 27), 29445256, 2, "Temperlay", true, true, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(12,55), false, LocalTime.of(13,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(12,30), false, LocalTime.of(12,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
-        <f>Pacientes!A16</f>
+        <f>Pacientes!B17</f>
         <v>tempPatient = new Patient("Olivia", "Perez", LocalDate.of(1952, 7, 7), 9234568, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B17" t="str">
@@ -2726,9 +2801,9 @@
         <v>tempPatient = new Patient("Olivia", "Perez", LocalDate.of(1952, 7, 7), 9234568, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(13,15), false, LocalTime.of(13,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(12,45), false, LocalTime.of(13,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="str">
-        <f>Pacientes!A17</f>
+        <f>Pacientes!B18</f>
         <v>tempPatient = new Patient("Andres", "Maldini", LocalDate.of(1981, 1, 19), 28567532, 1, "Banfield", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B18" t="str">
@@ -2750,9 +2825,9 @@
         <v>tempPatient = new Patient("Andres", "Maldini", LocalDate.of(1981, 1, 19), 28567532, 1, "Banfield", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(13,30), false, LocalTime.of(13,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(13,0), false, LocalTime.of(13,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="str">
-        <f>Pacientes!A18</f>
+        <f>Pacientes!B19</f>
         <v>tempPatient = new Patient("Sebastian", "Titolo", LocalDate.of(1980, 7, 3), 26123982, 1, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B19" t="str">
@@ -2774,9 +2849,9 @@
         <v>tempPatient = new Patient("Sebastian", "Titolo", LocalDate.of(1980, 7, 3), 26123982, 1, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(13,45), false, LocalTime.of(14,5),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(13,15), true, LocalTime.of(13,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
-        <f>Pacientes!A19</f>
+        <f>Pacientes!B20</f>
         <v>tempPatient = new Patient("Camila", "Ensilla", LocalDate.of(1990, 10, 2), 37091840, 2, "Lomas", false, false, true, false, true); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B20" t="str">
@@ -2798,9 +2873,9 @@
         <v>tempPatient = new Patient("Camila", "Ensilla", LocalDate.of(1990, 10, 2), 37091840, 2, "Lomas", false, false, true, false, true); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(14,5), false, LocalTime.of(14,20),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(13,30), true, LocalTime.of(13,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
-        <f>Pacientes!A20</f>
+        <f>Pacientes!B21</f>
         <v>tempPatient = new Patient("Roberto", "Burgos", LocalDate.of(1982, 7, 7), 290911112, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B21" t="str">
@@ -2822,9 +2897,9 @@
         <v>tempPatient = new Patient("Roberto", "Burgos", LocalDate.of(1982, 7, 7), 290911112, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(14,20), false, LocalTime.of(14,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(13,45), false, LocalTime.of(14,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
-        <f>Pacientes!A21</f>
+        <f>Pacientes!B22</f>
         <v>tempPatient = new Patient("Hugo", "Fernandez", LocalDate.of(1977, 9, 10), 25763201, 1, "CABA", true, true, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B22" t="str">
@@ -2846,9 +2921,9 @@
         <v>tempPatient = new Patient("Hugo", "Fernandez", LocalDate.of(1977, 9, 10), 25763201, 1, "CABA", true, true, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(14,45), false, LocalTime.of(15,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(14,0), false, LocalTime.of(14,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
-        <f>Pacientes!A22</f>
+        <f>Pacientes!B23</f>
         <v>tempPatient = new Patient("German", "Castro", LocalDate.of(1967, 1, 28), 18888881, 1, "Lomas", true, true,true, true, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B23" t="str">
@@ -2870,9 +2945,9 @@
         <v>tempPatient = new Patient("German", "Castro", LocalDate.of(1967, 1, 28), 18888881, 1, "Lomas", true, true,true, true, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(15,0), false, LocalTime.of(15,20),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(14,15), false, LocalTime.of(14,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="str">
-        <f>Pacientes!A23</f>
+        <f>Pacientes!B24</f>
         <v>tempPatient = new Patient("Sebastian", "Palmiero", LocalDate.of(1979, 9, 10), 261117625, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B24" t="str">
@@ -2894,9 +2969,9 @@
         <v>tempPatient = new Patient("Sebastian", "Palmiero", LocalDate.of(1979, 9, 10), 261117625, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(15,20), false, LocalTime.of(15,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(14,30), true, LocalTime.of(14,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="str">
-        <f>Pacientes!A24</f>
+        <f>Pacientes!B25</f>
         <v>tempPatient = new Patient("Gustavo", "Bermudez", LocalDate.of(1986, 6, 28), 33554109, 1, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B25" t="str">
@@ -2918,9 +2993,9 @@
         <v>tempPatient = new Patient("Gustavo", "Bermudez", LocalDate.of(1986, 6, 28), 33554109, 1, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(15,30), false, LocalTime.of(15,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(14,45), false, LocalTime.of(15,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
-        <f>Pacientes!A25</f>
+        <f>Pacientes!B26</f>
         <v>tempPatient = new Patient("Anabela", "Lucia", LocalDate.of(1983, 8, 12), 31311256, 1, "Temperley", false, false, false, true, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B26" t="str">
@@ -2942,9 +3017,9 @@
         <v>tempPatient = new Patient("Anabela", "Lucia", LocalDate.of(1983, 8, 12), 31311256, 1, "Temperley", false, false, false, true, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(15,45), false, LocalTime.of(16,5),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(15,0), false, LocalTime.of(15,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
-        <f>Pacientes!A26</f>
+        <f>Pacientes!B27</f>
         <v>tempPatient = new Patient("Sebastian", "Saccani", LocalDate.of(1985, 12, 12), 30137911, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B27" t="str">
@@ -2966,9 +3041,9 @@
         <v>tempPatient = new Patient("Sebastian", "Saccani", LocalDate.of(1985, 12, 12), 30137911, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(16,5), false, LocalTime.of(16,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(15,15), false, LocalTime.of(15,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
-        <f>Pacientes!A27</f>
+        <f>Pacientes!B28</f>
         <v>tempPatient = new Patient("Natalia", "Saccani", LocalDate.of(1989, 6, 13), 36009272, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B28" t="str">
@@ -2990,9 +3065,9 @@
         <v>tempPatient = new Patient("Natalia", "Saccani", LocalDate.of(1989, 6, 13), 36009272, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(16,15), false, LocalTime.of(16,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(15,30), false, LocalTime.of(15,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
-        <f>Pacientes!A28</f>
+        <f>Pacientes!B29</f>
         <v>tempPatient = new Patient("Natalia", "Damele", LocalDate.of(1990, 1, 13), 40192827, 1, "Lanus", false, false, false, true, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B29" t="str">
@@ -3014,9 +3089,9 @@
         <v>tempPatient = new Patient("Natalia", "Damele", LocalDate.of(1990, 1, 13), 40192827, 1, "Lanus", false, false, false, true, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(16,30), false, LocalTime.of(16,50),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(15,45), false, LocalTime.of(16,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="str">
-        <f>Pacientes!A29</f>
+        <f>Pacientes!B30</f>
         <v>tempPatient = new Patient("Eliana", "Matera", LocalDate.of(1994, 11, 19), 45029126, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B30" t="str">
@@ -3038,9 +3113,9 @@
         <v>tempPatient = new Patient("Eliana", "Matera", LocalDate.of(1994, 11, 19), 45029126, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(16,50), false, LocalTime.of(17,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(16,0), true, LocalTime.of(16,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="str">
-        <f>Pacientes!A30</f>
+        <f>Pacientes!B31</f>
         <v>tempPatient = new Patient("Florencia", "Persiani", LocalDate.of(1986, 9, 20), 33245927, 2, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B31" t="str">
@@ -3062,9 +3137,9 @@
         <v>tempPatient = new Patient("Florencia", "Persiani", LocalDate.of(1986, 9, 20), 33245927, 2, "Lomas", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(17,0), false, LocalTime.of(17,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(16,15), false, LocalTime.of(16,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="str">
-        <f>Pacientes!A31</f>
+        <f>Pacientes!B32</f>
         <v>tempPatient = new Patient("Florencia", "De Lucca", LocalDate.of(1991, 5, 12), 37726189, 2, "Lanus", false, false, false, true, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B32" t="str">
@@ -3086,9 +3161,9 @@
         <v>tempPatient = new Patient("Florencia", "De Lucca", LocalDate.of(1991, 5, 12), 37726189, 2, "Lanus", false, false, false, true, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(17,15), false, LocalTime.of(17,25),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(16,30), false, LocalTime.of(16,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="str">
-        <f>Pacientes!A32</f>
+        <f>Pacientes!B33</f>
         <v>tempPatient = new Patient("Norma", "Ponce", LocalDate.of(1968, 5, 4), 13916645, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B33" t="str">
@@ -3110,9 +3185,9 @@
         <v>tempPatient = new Patient("Norma", "Ponce", LocalDate.of(1968, 5, 4), 13916645, 1, "CABA", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(17,25), false, LocalTime.of(17,40),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(16,45), false, LocalTime.of(17,0),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="str">
-        <f>Pacientes!A33</f>
+        <f>Pacientes!B34</f>
         <v>tempPatient = new Patient("Florencia", "Salamanca", LocalDate.of(1995, 6, 13), 46782722, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B34" t="str">
@@ -3134,9 +3209,9 @@
         <v>tempPatient = new Patient("Florencia", "Salamanca", LocalDate.of(1995, 6, 13), 46782722, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(17,40), false, LocalTime.of(17,55),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(17,0), false, LocalTime.of(17,15),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="str">
-        <f>Pacientes!A34</f>
+        <f>Pacientes!B35</f>
         <v>tempPatient = new Patient("Vanesa", "Apodaca", LocalDate.of(1982, 5, 14), 29786687, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B35" t="str">
@@ -3158,9 +3233,9 @@
         <v>tempPatient = new Patient("Vanesa", "Apodaca", LocalDate.of(1982, 5, 14), 29786687, 2, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(17,55), false, LocalTime.of(18,10),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(17,15), false, LocalTime.of(17,30),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="str">
-        <f>Pacientes!A35</f>
+        <f>Pacientes!B36</f>
         <v>tempPatient = new Patient("Gabriel", "Perez", LocalDate.of(1988, 3, 27), 35781115, 1, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B36" t="str">
@@ -3182,9 +3257,9 @@
         <v>tempPatient = new Patient("Gabriel", "Perez", LocalDate.of(1988, 3, 27), 35781115, 1, "Lanus", true, false, false, false, false); patientRepository.save(tempPatient);tempAppointment = new Appointment(LocalDate.of(2021, 6, 1), LocalTime.of(18,10), false, LocalTime.of(18,25),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);tempAppointment = new Appointment(LocalDate.of(2021, 6, 2), LocalTime.of(17,30), false, LocalTime.of(17,45),tempClinica, tempPatient, true, false);appointmentRepository.save(tempAppointment);</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="str">
-        <f>Pacientes!A36</f>
+        <f>Pacientes!B37</f>
         <v>tempPatient = new Patient("Gonzalo", "Marcec", LocalDate.of(1984, 7, 10), 31766985, 1, "Lanus", true, false,false, false, false); patientRepository.save(tempPatient);</v>
       </c>
       <c r="B37" t="str">
@@ -3219,29 +3294,29 @@
       <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.41796875" customWidth="1"/>
+    <col min="2" max="2" width="4.83984375" customWidth="1"/>
+    <col min="3" max="3" width="57.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="45" t="s">
+    <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C1" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="46"/>
-    </row>
-    <row r="2" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="50" t="s">
+      <c r="D1" s="56"/>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C2" s="53" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C3" s="34" t="s">
         <v>224</v>
       </c>
@@ -3249,7 +3324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C4" s="36" t="s">
         <v>222</v>
       </c>
@@ -3257,25 +3332,25 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="58" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="59"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
     </row>
-    <row r="7" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="61"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C8" s="34" t="s">
         <v>224</v>
       </c>
@@ -3283,7 +3358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="42.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="42.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="4" t="s">
         <v>234</v>
       </c>
@@ -3291,29 +3366,29 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="59"/>
+      <c r="D11" s="58"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="52" t="s">
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="61" t="s">
         <v>216</v>
       </c>
-      <c r="D12" s="53"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="62"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C13" s="34" t="s">
         <v>224</v>
       </c>
@@ -3321,7 +3396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="4" t="s">
         <v>215</v>
       </c>
@@ -3331,27 +3406,27 @@
       <c r="E14" s="32"/>
       <c r="F14" s="32"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="54"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="52" t="s">
+    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="61" t="s">
         <v>226</v>
       </c>
-      <c r="D17" s="53"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="62"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C18" s="34" t="s">
         <v>224</v>
       </c>
@@ -3359,7 +3434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="4" t="s">
         <v>217</v>
       </c>
@@ -3369,25 +3444,25 @@
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="9"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="54" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="54"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="55" t="s">
+      <c r="D21" s="63"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="D22" s="56"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="34" t="s">
@@ -3399,7 +3474,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="9" t="s">
         <v>219</v>
       </c>
@@ -3407,29 +3482,29 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="1"/>
       <c r="D25" s="33"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="54" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26" s="63" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="54"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
     </row>
-    <row r="27" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="61" t="s">
         <v>235</v>
       </c>
-      <c r="D27" s="53"/>
+      <c r="D27" s="62"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C28" s="34" t="s">
         <v>224</v>
       </c>
@@ -3437,7 +3512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="4" t="s">
         <v>221</v>
       </c>
@@ -3445,27 +3520,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E30" s="32"/>
       <c r="F30" s="32"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="46"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="50" t="s">
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C32" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="51"/>
-    </row>
-    <row r="33" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="69"/>
+    </row>
+    <row r="33" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C33" s="34" t="s">
         <v>224</v>
       </c>
@@ -3473,7 +3548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C34" s="36" t="s">
         <v>231</v>
       </c>
@@ -3483,20 +3558,20 @@
       <c r="E34" s="32"/>
       <c r="F34" s="32"/>
     </row>
-    <row r="35" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="45" t="s">
+    <row r="35" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="36" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C36" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="D36" s="46"/>
-    </row>
-    <row r="37" spans="3:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="47" t="s">
+      <c r="D36" s="56"/>
+    </row>
+    <row r="37" spans="3:6" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37" s="66" t="s">
         <v>241</v>
       </c>
-      <c r="D37" s="48"/>
-    </row>
-    <row r="38" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="67"/>
+    </row>
+    <row r="38" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C38" s="34" t="s">
         <v>224</v>
       </c>
@@ -3504,7 +3579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="3:6" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C39" s="36" t="s">
         <v>237</v>
       </c>
@@ -3512,20 +3587,20 @@
         <v>238</v>
       </c>
     </row>
-    <row r="40" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="45" t="s">
+    <row r="40" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="41" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C41" s="55" t="s">
         <v>242</v>
       </c>
-      <c r="D41" s="49"/>
-    </row>
-    <row r="42" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="50" t="s">
+      <c r="D41" s="68"/>
+    </row>
+    <row r="42" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C42" s="53" t="s">
         <v>243</v>
       </c>
-      <c r="D42" s="51"/>
-    </row>
-    <row r="43" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="69"/>
+    </row>
+    <row r="43" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C43" s="34" t="s">
         <v>224</v>
       </c>
@@ -3533,7 +3608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="3:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:6" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C44" s="36" t="s">
         <v>239</v>
       </c>
@@ -3543,17 +3618,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C41:D41"/>
@@ -3561,6 +3625,17 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3575,21 +3650,21 @@
       <selection activeCell="B42" sqref="B42:P42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="44" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.578125" customWidth="1"/>
+    <col min="10" max="18" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="44" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19"/>
       <c r="B1" s="13" t="s">
         <v>41</v>
@@ -3607,11 +3682,11 @@
         <f>TIME(0,15,0)</f>
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>142</v>
       </c>
@@ -3745,7 +3820,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3779,7 +3854,7 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3816,7 +3891,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -3862,7 +3937,7 @@
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="22" t="s">
         <v>109</v>
       </c>
@@ -3911,7 +3986,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="22" t="s">
         <v>110</v>
       </c>
@@ -3963,7 +4038,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="22" t="s">
         <v>111</v>
       </c>
@@ -4018,7 +4093,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="22" t="s">
         <v>112</v>
       </c>
@@ -4076,7 +4151,7 @@
       </c>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="22" t="s">
         <v>113</v>
       </c>
@@ -4137,7 +4212,7 @@
         <v>0.44791666666666702</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="22" t="s">
         <v>114</v>
       </c>
@@ -4202,7 +4277,7 @@
         <v>0.45833333333333298</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="22" t="s">
         <v>115</v>
       </c>
@@ -4271,7 +4346,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="22" t="s">
         <v>116</v>
       </c>
@@ -4344,7 +4419,7 @@
         <v>0.47916666666666702</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="22" t="s">
         <v>117</v>
       </c>
@@ -4421,7 +4496,7 @@
         <v>0.48958333333333398</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="22" t="s">
         <v>118</v>
       </c>
@@ -4502,7 +4577,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="22" t="s">
         <v>119</v>
       </c>
@@ -4587,7 +4662,7 @@
         <v>0.51041666666666696</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="22" t="s">
         <v>120</v>
       </c>
@@ -4676,7 +4751,7 @@
         <v>0.52083333333333404</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="22" t="s">
         <v>121</v>
       </c>
@@ -4769,7 +4844,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="22" t="s">
         <v>122</v>
       </c>
@@ -4866,7 +4941,7 @@
         <v>0.54166666666666696</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="22" t="s">
         <v>123</v>
       </c>
@@ -4967,7 +5042,7 @@
         <v>0.55208333333333404</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="22" t="s">
         <v>124</v>
       </c>
@@ -5072,7 +5147,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="22" t="s">
         <v>125</v>
       </c>
@@ -5181,7 +5256,7 @@
         <v>0.57291666666666696</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="22" t="s">
         <v>126</v>
       </c>
@@ -5294,7 +5369,7 @@
         <v>0.58333333333333404</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="22" t="s">
         <v>127</v>
       </c>
@@ -5411,7 +5486,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="22" t="s">
         <v>128</v>
       </c>
@@ -5532,7 +5607,7 @@
         <v>0.60416666666666696</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="22" t="s">
         <v>129</v>
       </c>
@@ -5657,7 +5732,7 @@
         <v>0.61458333333333404</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="22" t="s">
         <v>130</v>
       </c>
@@ -5786,7 +5861,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="22" t="s">
         <v>131</v>
       </c>
@@ -5919,7 +5994,7 @@
         <v>0.63541666666666696</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="22" t="s">
         <v>132</v>
       </c>
@@ -6056,7 +6131,7 @@
         <v>0.64583333333333404</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="22" t="s">
         <v>133</v>
       </c>
@@ -6197,7 +6272,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="22" t="s">
         <v>134</v>
       </c>
@@ -6342,7 +6417,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="22" t="s">
         <v>135</v>
       </c>
@@ -6491,7 +6566,7 @@
         <v>0.67708333333333404</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="22" t="s">
         <v>136</v>
       </c>
@@ -6644,7 +6719,7 @@
         <v>0.687500000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -6801,7 +6876,7 @@
         <v>0.69791666666666696</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -6962,7 +7037,7 @@
         <v>0.70833333333333404</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -7127,7 +7202,7 @@
         <v>0.718750000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -7296,7 +7371,7 @@
         <v>0.72916666666666696</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -7469,47 +7544,47 @@
         <v>0.73958333333333404</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B41" s="68" t="s">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="70" t="s">
         <v>248</v>
       </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="68"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68"/>
-      <c r="Q41" s="68"/>
-    </row>
-    <row r="42" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="68" t="s">
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="70"/>
+      <c r="M41" s="70"/>
+      <c r="N41" s="70"/>
+      <c r="O41" s="70"/>
+      <c r="P41" s="70"/>
+      <c r="Q41" s="70"/>
+    </row>
+    <row r="42" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
-    </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B43" s="69" t="s">
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="70"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="70"/>
+      <c r="M42" s="70"/>
+      <c r="N42" s="70"/>
+      <c r="O42" s="70"/>
+      <c r="P42" s="70"/>
+    </row>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="44" t="s">
         <v>250</v>
       </c>
     </row>
@@ -7527,26 +7602,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AAC928-D5F2-4412-8D8F-A754DC5B9F83}">
   <dimension ref="A1:AT38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K1048576"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="18.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="141.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="46" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.68359375" customWidth="1"/>
+    <col min="7" max="7" width="9.83984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.47265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="119.62890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="13" max="20" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="46" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19"/>
       <c r="B1" s="13" t="s">
         <v>41</v>
@@ -7564,12 +7641,12 @@
         <f>TIME(0,15,0)</f>
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="H1" s="72"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="74"/>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="H1" s="47"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="49"/>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>142</v>
       </c>
@@ -7591,19 +7668,19 @@
       <c r="G2" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="J2" s="70" t="s">
+      <c r="J2" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="L2" s="71" t="s">
+      <c r="L2" s="46" t="s">
         <v>96</v>
       </c>
       <c r="M2" s="16" t="s">
@@ -7709,7 +7786,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -7751,7 +7828,7 @@
       </c>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -7796,7 +7873,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -7850,7 +7927,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -7907,7 +7984,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -7967,7 +8044,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -8030,7 +8107,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -8096,7 +8173,7 @@
       </c>
       <c r="R9" s="6"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -8165,7 +8242,7 @@
         <v>0.4583333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -8238,7 +8315,7 @@
         <v>0.46874999999999967</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -8315,7 +8392,7 @@
         <v>0.4826388888888889</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -8396,7 +8473,7 @@
         <v>0.48611111111111144</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -8481,7 +8558,7 @@
         <v>0.50000000000000067</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -8570,7 +8647,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -8663,7 +8740,7 @@
         <v>0.5243055555555558</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -8760,7 +8837,7 @@
         <v>0.5381944444444452</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -8861,7 +8938,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -8966,7 +9043,7 @@
         <v>0.56250000000000033</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -9075,7 +9152,7 @@
         <v>0.57291666666666741</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -9188,7 +9265,7 @@
         <v>0.58680555555555558</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -9305,7 +9382,7 @@
         <v>0.59722222222222254</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -9426,7 +9503,7 @@
         <v>0.61458333333333404</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -9551,7 +9628,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -9680,7 +9757,7 @@
         <v>0.63888888888888917</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -9813,7 +9890,7 @@
         <v>0.64583333333333404</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -9950,7 +10027,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>131</v>
       </c>
@@ -10091,7 +10168,7 @@
         <v>0.67013888888888917</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -10236,7 +10313,7 @@
         <v>0.67708333333333404</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -10385,7 +10462,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -10538,7 +10615,7 @@
         <v>0.70138888888888917</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -10695,7 +10772,7 @@
         <v>0.70833333333333404</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -10856,7 +10933,7 @@
         <v>0.718750000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -11021,7 +11098,7 @@
         <v>0.72569444444444475</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -11190,7 +11267,7 @@
         <v>0.73611111111111183</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -11363,7 +11440,7 @@
         <v>0.74652777777777879</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -11540,7 +11617,7 @@
         <v>0.75694444444444475</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -11735,21 +11812,21 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="11" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="148.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="45" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="148.41796875" hidden="1" customWidth="1"/>
+    <col min="11" max="19" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="45" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19"/>
       <c r="B1" s="13" t="s">
         <v>41</v>
@@ -11767,12 +11844,12 @@
         <f>TIME(0,15,0)</f>
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="74"/>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="49"/>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>142</v>
       </c>
@@ -11791,16 +11868,16 @@
       <c r="F2" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="J2" s="70" t="s">
+      <c r="J2" s="45" t="s">
         <v>247</v>
       </c>
       <c r="K2" s="16" t="s">
@@ -11909,7 +11986,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -11946,7 +12023,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -11986,7 +12063,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -12035,7 +12112,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -12087,7 +12164,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="20" t="s">
         <v>110</v>
       </c>
@@ -12142,7 +12219,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -12200,7 +12277,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -12261,7 +12338,7 @@
       </c>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -12325,7 +12402,7 @@
         <v>0.44791666666666702</v>
       </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -12393,7 +12470,7 @@
         <v>0.45833333333333298</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="20" t="s">
         <v>115</v>
       </c>
@@ -12465,7 +12542,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -12541,7 +12618,7 @@
         <v>0.47916666666666702</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="20" t="s">
         <v>117</v>
       </c>
@@ -12621,7 +12698,7 @@
         <v>0.48958333333333398</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -12705,7 +12782,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -12793,7 +12870,7 @@
         <v>0.51041666666666696</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -12885,7 +12962,7 @@
         <v>0.52083333333333404</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -12981,7 +13058,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -13081,7 +13158,7 @@
         <v>0.54166666666666696</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="20" t="s">
         <v>123</v>
       </c>
@@ -13185,7 +13262,7 @@
         <v>0.55208333333333404</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="20" t="s">
         <v>124</v>
       </c>
@@ -13293,7 +13370,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -13405,7 +13482,7 @@
         <v>0.57291666666666696</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -13521,7 +13598,7 @@
         <v>0.58333333333333404</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -13641,7 +13718,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="20" t="s">
         <v>128</v>
       </c>
@@ -13765,7 +13842,7 @@
         <v>0.60416666666666696</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -13893,7 +13970,7 @@
         <v>0.61458333333333404</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -14025,7 +14102,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>131</v>
       </c>
@@ -14161,7 +14238,7 @@
         <v>0.63541666666666696</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -14301,7 +14378,7 @@
         <v>0.64583333333333404</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -14445,7 +14522,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="20" t="s">
         <v>134</v>
       </c>
@@ -14593,7 +14670,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -14745,7 +14822,7 @@
         <v>0.67708333333333404</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -14901,7 +14978,7 @@
         <v>0.687500000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -15061,7 +15138,7 @@
         <v>0.69791666666666696</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -15225,7 +15302,7 @@
         <v>0.70833333333333404</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -15393,7 +15470,7 @@
         <v>0.718750000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -15565,7 +15642,7 @@
         <v>0.72916666666666696</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -15755,19 +15832,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="41" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19"/>
       <c r="B1" s="13" t="s">
         <v>41</v>
@@ -15786,7 +15863,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>142</v>
       </c>
@@ -15911,7 +15988,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -15933,7 +16010,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -15958,7 +16035,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -15992,7 +16069,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -16029,7 +16106,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -16069,7 +16146,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -16112,7 +16189,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -16158,7 +16235,7 @@
       </c>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -16207,7 +16284,7 @@
         <v>0.44791666666666702</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -16260,7 +16337,7 @@
         <v>0.45833333333333298</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -16317,7 +16394,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -16378,7 +16455,7 @@
         <v>0.47916666666666702</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -16443,7 +16520,7 @@
         <v>0.48958333333333398</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -16512,7 +16589,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -16585,7 +16662,7 @@
         <v>0.51041666666666696</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -16662,7 +16739,7 @@
         <v>0.52083333333333404</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -16743,7 +16820,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -16828,7 +16905,7 @@
         <v>0.54166666666666696</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -16917,7 +16994,7 @@
         <v>0.55208333333333404</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -17010,7 +17087,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -17107,7 +17184,7 @@
         <v>0.57291666666666696</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -17208,7 +17285,7 @@
         <v>0.58333333333333404</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -17313,7 +17390,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -17422,7 +17499,7 @@
         <v>0.60416666666666696</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -17535,7 +17612,7 @@
         <v>0.61458333333333404</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -17652,7 +17729,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>131</v>
       </c>
@@ -17773,7 +17850,7 @@
         <v>0.63541666666666696</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -17898,7 +17975,7 @@
         <v>0.64583333333333404</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -18027,7 +18104,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -18160,7 +18237,7 @@
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -18297,7 +18374,7 @@
         <v>0.67708333333333404</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -18438,7 +18515,7 @@
         <v>0.687500000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -18583,7 +18660,7 @@
         <v>0.69791666666666696</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -18732,7 +18809,7 @@
         <v>0.70833333333333404</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -18885,7 +18962,7 @@
         <v>0.718750000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -19042,7 +19119,7 @@
         <v>0.72916666666666696</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -19220,30 +19297,30 @@
       <selection pane="bottomRight" activeCell="A49" sqref="A49:B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.68359375" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="27" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="49" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="39" max="49" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19"/>
       <c r="B1" s="13" t="s">
         <v>41</v>
@@ -19305,7 +19382,7 @@
       <c r="AV1" s="24"/>
       <c r="AW1" s="24"/>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>142</v>
       </c>
@@ -19454,7 +19531,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="24" t="s">
         <v>23</v>
       </c>
@@ -19606,7 +19683,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="24" t="s">
         <v>24</v>
       </c>
@@ -19760,7 +19837,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="24" t="s">
         <v>108</v>
       </c>
@@ -19915,7 +19992,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="24" t="s">
         <v>109</v>
       </c>
@@ -20071,7 +20148,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="26" t="s">
         <v>110</v>
       </c>
@@ -20227,7 +20304,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="29" t="s">
         <v>178</v>
       </c>
@@ -20385,7 +20462,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="24" t="s">
         <v>111</v>
       </c>
@@ -20544,7 +20621,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="24" t="s">
         <v>112</v>
       </c>
@@ -20704,7 +20781,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="24" t="s">
         <v>113</v>
       </c>
@@ -20865,7 +20942,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="24" t="s">
         <v>114</v>
       </c>
@@ -21027,7 +21104,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="29" t="s">
         <v>168</v>
       </c>
@@ -21190,7 +21267,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="26" t="s">
         <v>115</v>
       </c>
@@ -21354,7 +21431,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="24" t="s">
         <v>116</v>
       </c>
@@ -21519,7 +21596,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="26" t="s">
         <v>117</v>
       </c>
@@ -21685,7 +21762,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="24" t="s">
         <v>118</v>
       </c>
@@ -21852,7 +21929,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="29" t="s">
         <v>169</v>
       </c>
@@ -22019,7 +22096,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="24" t="s">
         <v>119</v>
       </c>
@@ -22188,7 +22265,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="24" t="s">
         <v>120</v>
       </c>
@@ -22358,7 +22435,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="24" t="s">
         <v>121</v>
       </c>
@@ -22529,7 +22606,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="24" t="s">
         <v>122</v>
       </c>
@@ -22701,7 +22778,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="29" t="s">
         <v>170</v>
       </c>
@@ -22874,7 +22951,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="26" t="s">
         <v>123</v>
       </c>
@@ -23048,7 +23125,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="26" t="s">
         <v>124</v>
       </c>
@@ -23223,7 +23300,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="24" t="s">
         <v>125</v>
       </c>
@@ -23399,7 +23476,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="24" t="s">
         <v>126</v>
       </c>
@@ -23576,7 +23653,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="29" t="s">
         <v>172</v>
       </c>
@@ -23754,7 +23831,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="24" t="s">
         <v>127</v>
       </c>
@@ -23933,7 +24010,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="26" t="s">
         <v>128</v>
       </c>
@@ -24113,7 +24190,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="24" t="s">
         <v>129</v>
       </c>
@@ -24294,7 +24371,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="24" t="s">
         <v>130</v>
       </c>
@@ -24476,7 +24553,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="29" t="s">
         <v>174</v>
       </c>
@@ -24659,7 +24736,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="24" t="s">
         <v>131</v>
       </c>
@@ -24843,7 +24920,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="24" t="s">
         <v>132</v>
       </c>
@@ -25028,7 +25105,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="24" t="s">
         <v>133</v>
       </c>
@@ -25214,7 +25291,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="26" t="s">
         <v>134</v>
       </c>
@@ -25401,7 +25478,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="29" t="s">
         <v>175</v>
       </c>
@@ -25589,7 +25666,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="24" t="s">
         <v>135</v>
       </c>
@@ -25778,7 +25855,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="24" t="s">
         <v>136</v>
       </c>
@@ -25968,7 +26045,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="24" t="s">
         <v>137</v>
       </c>
@@ -26159,7 +26236,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="24" t="s">
         <v>138</v>
       </c>
@@ -26351,7 +26428,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="24" t="s">
         <v>139</v>
       </c>
@@ -26544,7 +26621,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="24" t="s">
         <v>140</v>
       </c>
@@ -26738,7 +26815,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="24" t="s">
         <v>141</v>
       </c>
@@ -26933,29 +27010,29 @@
         <v>0.77083333333333293</v>
       </c>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A48" s="62" t="s">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="71" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="62"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="63" t="s">
+      <c r="B48" s="71"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="B49" s="63"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="64" t="s">
+      <c r="B49" s="72"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="B50" s="65"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="66" t="s">
+      <c r="B50" s="74"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="B51" s="66"/>
+      <c r="B51" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -26980,20 +27057,20 @@
       <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.68359375" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="16" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="42" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="19"/>
       <c r="B1" s="13" t="s">
         <v>41</v>
@@ -27048,7 +27125,7 @@
       <c r="AO1" s="24"/>
       <c r="AP1" s="24"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
         <v>142</v>
       </c>
@@ -27176,7 +27253,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="24" t="s">
         <v>23</v>
       </c>
@@ -27307,7 +27384,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="24" t="s">
         <v>24</v>
       </c>
@@ -27440,7 +27517,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="24" t="s">
         <v>108</v>
       </c>
@@ -27574,7 +27651,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="24" t="s">
         <v>109</v>
       </c>
@@ -27709,7 +27786,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="24" t="s">
         <v>110</v>
       </c>
@@ -27845,7 +27922,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="24" t="s">
         <v>111</v>
       </c>
@@ -27982,7 +28059,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="24" t="s">
         <v>112</v>
       </c>
@@ -28120,7 +28197,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="24" t="s">
         <v>113</v>
       </c>
@@ -28259,7 +28336,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="24" t="s">
         <v>114</v>
       </c>
@@ -28399,7 +28476,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="24" t="s">
         <v>115</v>
       </c>
@@ -28540,7 +28617,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="24" t="s">
         <v>116</v>
       </c>
@@ -28682,7 +28759,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="24" t="s">
         <v>117</v>
       </c>
@@ -28825,7 +28902,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="24" t="s">
         <v>118</v>
       </c>
@@ -28969,7 +29046,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:42" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" s="42" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="38" t="s">
         <v>119</v>
       </c>
@@ -29114,7 +29191,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="24" t="s">
         <v>120</v>
       </c>
@@ -29260,7 +29337,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="24" t="s">
         <v>121</v>
       </c>
@@ -29407,7 +29484,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="24" t="s">
         <v>122</v>
       </c>
@@ -29555,7 +29632,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="24" t="s">
         <v>123</v>
       </c>
@@ -29704,7 +29781,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="24" t="s">
         <v>124</v>
       </c>
@@ -29854,7 +29931,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="24" t="s">
         <v>125</v>
       </c>
@@ -30005,7 +30082,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="24" t="s">
         <v>126</v>
       </c>
@@ -30157,7 +30234,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="24" t="s">
         <v>127</v>
       </c>
@@ -30310,7 +30387,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="30" t="s">
         <v>128</v>
       </c>
@@ -30464,7 +30541,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="31" t="s">
         <v>193</v>
       </c>
@@ -30618,7 +30695,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="24" t="s">
         <v>129</v>
       </c>
@@ -30773,7 +30850,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="24" t="s">
         <v>130</v>
       </c>
@@ -30929,7 +31006,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="24" t="s">
         <v>131</v>
       </c>
@@ -31086,7 +31163,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="24" t="s">
         <v>132</v>
       </c>
@@ -31244,7 +31321,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="24" t="s">
         <v>133</v>
       </c>
@@ -31403,7 +31480,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="30" t="s">
         <v>134</v>
       </c>
@@ -31563,7 +31640,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="31" t="s">
         <v>134</v>
       </c>
@@ -31723,7 +31800,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="24" t="s">
         <v>135</v>
       </c>
@@ -31884,7 +31961,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="24" t="s">
         <v>136</v>
       </c>
@@ -32046,7 +32123,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="24" t="s">
         <v>137</v>
       </c>
@@ -32209,7 +32286,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="24" t="s">
         <v>138</v>
       </c>
@@ -32373,7 +32450,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="24" t="s">
         <v>139</v>
       </c>
@@ -32538,7 +32615,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="24" t="s">
         <v>140</v>
       </c>
@@ -32704,7 +32781,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="24" t="s">
         <v>141</v>
       </c>
@@ -32871,33 +32948,33 @@
         <v>0.74652777777777757</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A43" s="62" t="s">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="71" t="s">
         <v>188</v>
       </c>
-      <c r="B43" s="62"/>
-    </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A44" s="63" t="s">
+      <c r="B43" s="71"/>
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="B44" s="63"/>
+      <c r="B44" s="72"/>
       <c r="G44" s="6">
         <f>E10-(B10+$G$1)</f>
         <v>3.4722222222219878E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A45" s="64" t="s">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="73" t="s">
         <v>190</v>
       </c>
-      <c r="B45" s="65"/>
-    </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A46" s="66" t="s">
+      <c r="B45" s="74"/>
+    </row>
+    <row r="46" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="B46" s="66"/>
+      <c r="B46" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -32913,195 +32990,328 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABED78B2-C549-4968-8087-F00418B9D012}">
-  <dimension ref="A1:A36"/>
+  <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="154.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="154.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="str">
+        <f>MID(B2,SEARCH("""",B2,1),(SEARCH("""",B2,SEARCH("""",B2,1)+1)+1)-SEARCH("""",B2,1))</f>
+        <v>"Julio"</v>
+      </c>
+      <c r="D2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I2">
+        <v>10664879</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>301</v>
+      </c>
+      <c r="L2" t="s">
+        <v>303</v>
+      </c>
+      <c r="M2" t="s">
+        <v>302</v>
+      </c>
+      <c r="N2" t="s">
+        <v>303</v>
+      </c>
+      <c r="O2" t="s">
+        <v>303</v>
+      </c>
+      <c r="P2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C14" si="0">MID(B3,SEARCH("""",B3,1),(SEARCH("""",B3,SEARCH("""",B3,1)+1)+1)-SEARCH("""",B3,1))</f>
+        <v>"Beatriz"</v>
+      </c>
+      <c r="D3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H3">
+        <v>9215788</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>301</v>
+      </c>
+      <c r="K3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L3" t="s">
+        <v>303</v>
+      </c>
+      <c r="M3" t="s">
+        <v>303</v>
+      </c>
+      <c r="N3" t="s">
+        <v>303</v>
+      </c>
+      <c r="O3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cristian"</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Victoria"</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Camila"</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Gabriela"</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Francisco"</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Emilio"</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Iris"</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Luciano"</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Alejo"</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Paula"</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Julio"</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -33119,6 +33329,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E4F2C5C2C688D4294DD0A7E4ED187A4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d8ff5051fae7958e87729961111201">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ee180031-54aa-4547-ae85-69ab37712938" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fff74c3b61c94382445f1fd2917e5df0" ns3:_="">
     <xsd:import namespace="ee180031-54aa-4547-ae85-69ab37712938"/>
@@ -33296,12 +33512,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F4D3E87-D9C3-4CF2-AFF5-95DABA850468}">
   <ds:schemaRefs>
@@ -33311,6 +33521,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBDC475-0F27-4861-89EC-4F8D2CA5B947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DE4F7D5-E079-443F-A2F6-B66290943DAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33326,13 +33545,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBDC475-0F27-4861-89EC-4F8D2CA5B947}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test Case 1 y 2 funcionando
Se configuraron los excel para generar los datos de los casos de prueba...
</commit_message>
<xml_diff>
--- a/Casos de prueba/Casos de prueba TFI.xlsx
+++ b/Casos de prueba/Casos de prueba TFI.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haria\Repositories\TFI-BackEnd\Casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F808304E-2665-40EA-AC6C-E949B7C41B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D6972B-B47F-43D3-BBC1-3F808233810E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" firstSheet="3" activeTab="4" xr2:uid="{E19D2194-C2B1-4B6D-9336-FDF693023F08}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="1" xr2:uid="{E19D2194-C2B1-4B6D-9336-FDF693023F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="10" r:id="rId2"/>
-    <sheet name="Todo en Hora" sheetId="4" r:id="rId3"/>
-    <sheet name="Caso 1(ETAs)" sheetId="3" r:id="rId4"/>
-    <sheet name="Caso 2(Cancelados 0.2)" sheetId="6" r:id="rId5"/>
-    <sheet name="Caso 3" sheetId="5" r:id="rId6"/>
-    <sheet name="Caso 4(ETAs) (Canc 0.2)" sheetId="8" r:id="rId7"/>
-    <sheet name="Caso 5(ETAs) (Adelantar)" sheetId="9" r:id="rId8"/>
-    <sheet name="Pacientes" sheetId="11" r:id="rId9"/>
-    <sheet name="Usuarios" sheetId="13" r:id="rId10"/>
-    <sheet name="CodeLineRunner" sheetId="12" r:id="rId11"/>
+    <sheet name="Creados" sheetId="14" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="10" r:id="rId3"/>
+    <sheet name="Todo en Hora" sheetId="4" r:id="rId4"/>
+    <sheet name="Caso 1(ETAs)" sheetId="3" r:id="rId5"/>
+    <sheet name="Caso 2(Cancelados 0.2)" sheetId="6" r:id="rId6"/>
+    <sheet name="Caso 3" sheetId="5" r:id="rId7"/>
+    <sheet name="Caso 4(ETAs) (Canc 0.2)" sheetId="8" r:id="rId8"/>
+    <sheet name="Caso 5(ETAs) (Adelantar)" sheetId="9" r:id="rId9"/>
+    <sheet name="Pacientes" sheetId="11" state="hidden" r:id="rId10"/>
+    <sheet name="Usuarios" sheetId="13" state="hidden" r:id="rId11"/>
+    <sheet name="CodeLineRunner" sheetId="12" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3523" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3535" uniqueCount="402">
   <si>
     <t>Operacion</t>
   </si>
@@ -1262,6 +1263,24 @@
   </si>
   <si>
     <t>App LocalTime</t>
+  </si>
+  <si>
+    <t>* El paciente con el turno de las 16:45 (caso1) selecciona la opción "Sala de Espera" en el menú principal.</t>
+  </si>
+  <si>
+    <t>Turno retrasado</t>
+  </si>
+  <si>
+    <t>Se muestran los datos del próximo turno al usuario, estando este retrasado.</t>
+  </si>
+  <si>
+    <t>* El paciente con el turno de las 16:45 (caso2) selecciona la opción "Sala de Espera" en el menú principal.</t>
+  </si>
+  <si>
+    <t>Durante el día 01-06-2021 los de turnos hasta las 16:30 se deben haber completado en hora, siendo este el escenario ideal.</t>
+  </si>
+  <si>
+    <t>Durante el día 02-06-2021 los turnos hasta el turno las 16:00 estarán completados, y con un acumulado de retraso de 45 minutos.</t>
   </si>
 </sst>
 </file>
@@ -1696,11 +1715,22 @@
     <xf numFmtId="20" fontId="5" fillId="12" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="5" fillId="12" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1708,19 +1738,16 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1738,19 +1765,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1771,11 +1795,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
@@ -2094,7 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28C3F43-2EA3-4F91-B792-718673B4B8A4}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2109,14 +2128,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
@@ -2171,14 +2190,14 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
@@ -2237,12 +2256,12 @@
         <v>198</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5" t="s">
@@ -2393,12 +2412,12 @@
         <v>199</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
@@ -2625,6 +2644,1692 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABED78B2-C549-4968-8087-F00418B9D012}">
+  <dimension ref="A1:O37"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="31.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.62890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.05078125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="146.05078125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" t="s">
+        <v>275</v>
+      </c>
+      <c r="O1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F2">
+        <v>10664879</v>
+      </c>
+      <c r="G2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H2" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2" t="s">
+        <v>263</v>
+      </c>
+      <c r="K2" t="s">
+        <v>264</v>
+      </c>
+      <c r="L2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M2" t="s">
+        <v>393</v>
+      </c>
+      <c r="O2" t="str">
+        <f>_xlfn.TEXTJOIN(",",,A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,)</f>
+        <v>tempPatient = new Patient("Julio", "Arias", LocalDate.of(1953,1, 17),10664879,Gender.MALE, "Lanus", false, true, false, false, false);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3">
+        <v>9215788</v>
+      </c>
+      <c r="G3" t="s">
+        <v>374</v>
+      </c>
+      <c r="H3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J3" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" t="s">
+        <v>264</v>
+      </c>
+      <c r="L3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M3" t="s">
+        <v>393</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O37" si="0">_xlfn.TEXTJOIN(",",,A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,)</f>
+        <v>tempPatient = new Patient("Beatriz", "Leguizamon", LocalDate.of(1955,6, 25),9215788,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4">
+        <v>30127532</v>
+      </c>
+      <c r="G4" t="s">
+        <v>375</v>
+      </c>
+      <c r="H4" t="s">
+        <v>280</v>
+      </c>
+      <c r="I4" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" t="s">
+        <v>264</v>
+      </c>
+      <c r="L4" t="s">
+        <v>264</v>
+      </c>
+      <c r="M4" t="s">
+        <v>393</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Cristian", "Vallarino", LocalDate.of(1983,2, 22),30127532,Gender.MALE, "Banfield", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F5">
+        <v>26742442</v>
+      </c>
+      <c r="G5" t="s">
+        <v>374</v>
+      </c>
+      <c r="H5" t="s">
+        <v>283</v>
+      </c>
+      <c r="I5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J5" t="s">
+        <v>264</v>
+      </c>
+      <c r="K5" t="s">
+        <v>264</v>
+      </c>
+      <c r="L5" t="s">
+        <v>264</v>
+      </c>
+      <c r="M5" t="s">
+        <v>393</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Victoria", "Arias", LocalDate.of(1980,1, 25),26742442,Gender.FEMALE, "Lomas", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6">
+        <v>30333982</v>
+      </c>
+      <c r="G6" t="s">
+        <v>374</v>
+      </c>
+      <c r="H6" t="s">
+        <v>283</v>
+      </c>
+      <c r="I6" t="s">
+        <v>264</v>
+      </c>
+      <c r="J6" t="s">
+        <v>264</v>
+      </c>
+      <c r="K6" t="s">
+        <v>263</v>
+      </c>
+      <c r="L6" t="s">
+        <v>264</v>
+      </c>
+      <c r="M6" t="s">
+        <v>393</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Camila", "Garcia", LocalDate.of(1982,7, 9),30333982,Gender.FEMALE, "Lomas", false, false, true, false, false);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7">
+        <v>28447445</v>
+      </c>
+      <c r="G7" t="s">
+        <v>374</v>
+      </c>
+      <c r="H7" t="s">
+        <v>292</v>
+      </c>
+      <c r="I7" t="s">
+        <v>263</v>
+      </c>
+      <c r="J7" t="s">
+        <v>264</v>
+      </c>
+      <c r="K7" t="s">
+        <v>264</v>
+      </c>
+      <c r="L7" t="s">
+        <v>264</v>
+      </c>
+      <c r="M7" t="s">
+        <v>393</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Gabriela", "Suarez", LocalDate.of(1981,11, 11),28447445,Gender.FEMALE, "CABA", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F8">
+        <v>25725839</v>
+      </c>
+      <c r="G8" t="s">
+        <v>375</v>
+      </c>
+      <c r="H8" t="s">
+        <v>292</v>
+      </c>
+      <c r="I8" t="s">
+        <v>263</v>
+      </c>
+      <c r="J8" t="s">
+        <v>263</v>
+      </c>
+      <c r="K8" t="s">
+        <v>264</v>
+      </c>
+      <c r="L8" t="s">
+        <v>264</v>
+      </c>
+      <c r="M8" t="s">
+        <v>393</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Francisco", "De Marco", LocalDate.of(1978,9, 10),25725839,Gender.MALE, "CABA", true, true, false, false, false);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C9" t="s">
+        <v>299</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9">
+        <v>20876091</v>
+      </c>
+      <c r="G9" t="s">
+        <v>375</v>
+      </c>
+      <c r="H9" t="s">
+        <v>283</v>
+      </c>
+      <c r="I9" t="s">
+        <v>263</v>
+      </c>
+      <c r="J9" t="s">
+        <v>263</v>
+      </c>
+      <c r="K9" t="s">
+        <v>263</v>
+      </c>
+      <c r="L9" t="s">
+        <v>263</v>
+      </c>
+      <c r="M9" t="s">
+        <v>393</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Emilio", "Dissi", LocalDate.of(1970,3, 3),20876091,Gender.MALE, "Lomas", true, true, true, true, false);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>304</v>
+      </c>
+      <c r="F10">
+        <v>33445775</v>
+      </c>
+      <c r="G10" t="s">
+        <v>374</v>
+      </c>
+      <c r="H10" t="s">
+        <v>262</v>
+      </c>
+      <c r="I10" t="s">
+        <v>263</v>
+      </c>
+      <c r="J10" t="s">
+        <v>264</v>
+      </c>
+      <c r="K10" t="s">
+        <v>264</v>
+      </c>
+      <c r="L10" t="s">
+        <v>264</v>
+      </c>
+      <c r="M10" t="s">
+        <v>393</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Iris", "De Ojo", LocalDate.of(1985,9, 1),33445775,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>291</v>
+      </c>
+      <c r="F11">
+        <v>22987456</v>
+      </c>
+      <c r="G11" t="s">
+        <v>375</v>
+      </c>
+      <c r="H11" t="s">
+        <v>283</v>
+      </c>
+      <c r="I11" t="s">
+        <v>263</v>
+      </c>
+      <c r="J11" t="s">
+        <v>264</v>
+      </c>
+      <c r="K11" t="s">
+        <v>264</v>
+      </c>
+      <c r="L11" t="s">
+        <v>264</v>
+      </c>
+      <c r="M11" t="s">
+        <v>393</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Luciano", "Lunga", LocalDate.of(1981,11, 11),22987456,Gender.MALE, "Lomas", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>309</v>
+      </c>
+      <c r="F12">
+        <v>29851753</v>
+      </c>
+      <c r="G12" t="s">
+        <v>375</v>
+      </c>
+      <c r="H12" t="s">
+        <v>310</v>
+      </c>
+      <c r="I12" t="s">
+        <v>264</v>
+      </c>
+      <c r="J12" t="s">
+        <v>264</v>
+      </c>
+      <c r="K12" t="s">
+        <v>264</v>
+      </c>
+      <c r="L12" t="s">
+        <v>263</v>
+      </c>
+      <c r="M12" t="s">
+        <v>393</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Alejo", "Perez", LocalDate.of(1982,2, 15),29851753,Gender.MALE, "Temperley", false, false, false, true, false);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>261</v>
+      </c>
+      <c r="F13">
+        <v>29356543</v>
+      </c>
+      <c r="G13" t="s">
+        <v>374</v>
+      </c>
+      <c r="H13" t="s">
+        <v>262</v>
+      </c>
+      <c r="I13" t="s">
+        <v>264</v>
+      </c>
+      <c r="J13" t="s">
+        <v>263</v>
+      </c>
+      <c r="K13" t="s">
+        <v>264</v>
+      </c>
+      <c r="L13" t="s">
+        <v>264</v>
+      </c>
+      <c r="M13" t="s">
+        <v>393</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Paula", "Perez", LocalDate.of(1980,2, 25),29356543,Gender.FEMALE, "Lanus", false, true, false, false, false);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>309</v>
+      </c>
+      <c r="F14">
+        <v>12615229</v>
+      </c>
+      <c r="G14" t="s">
+        <v>375</v>
+      </c>
+      <c r="H14" t="s">
+        <v>262</v>
+      </c>
+      <c r="I14" t="s">
+        <v>264</v>
+      </c>
+      <c r="J14" t="s">
+        <v>264</v>
+      </c>
+      <c r="K14" t="s">
+        <v>264</v>
+      </c>
+      <c r="L14" t="s">
+        <v>264</v>
+      </c>
+      <c r="M14" t="s">
+        <v>393</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Julio", "Sanchez", LocalDate.of(1955,5, 15),12615229,Gender.MALE, "Lanus", false, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" t="s">
+        <v>314</v>
+      </c>
+      <c r="C15" t="s">
+        <v>315</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>309</v>
+      </c>
+      <c r="F15">
+        <v>33153323</v>
+      </c>
+      <c r="G15" t="s">
+        <v>374</v>
+      </c>
+      <c r="H15" t="s">
+        <v>262</v>
+      </c>
+      <c r="I15" t="s">
+        <v>264</v>
+      </c>
+      <c r="J15" t="s">
+        <v>264</v>
+      </c>
+      <c r="K15" t="s">
+        <v>264</v>
+      </c>
+      <c r="L15" t="s">
+        <v>264</v>
+      </c>
+      <c r="M15" t="s">
+        <v>393</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Laura", "Bonilla", LocalDate.of(1984,5, 15),33153323,Gender.FEMALE, "Lanus", false, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>316</v>
+      </c>
+      <c r="B16" t="s">
+        <v>317</v>
+      </c>
+      <c r="C16" t="s">
+        <v>286</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F16">
+        <v>29445256</v>
+      </c>
+      <c r="G16" t="s">
+        <v>374</v>
+      </c>
+      <c r="H16" t="s">
+        <v>319</v>
+      </c>
+      <c r="I16" t="s">
+        <v>263</v>
+      </c>
+      <c r="J16" t="s">
+        <v>263</v>
+      </c>
+      <c r="K16" t="s">
+        <v>264</v>
+      </c>
+      <c r="L16" t="s">
+        <v>264</v>
+      </c>
+      <c r="M16" t="s">
+        <v>393</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Andrea", "Gonzales", LocalDate.of(1982,2, 27),29445256,Gender.FEMALE, "Temperlay", true, true, false, false, false);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>320</v>
+      </c>
+      <c r="B17" t="s">
+        <v>308</v>
+      </c>
+      <c r="C17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>322</v>
+      </c>
+      <c r="F17">
+        <v>9234568</v>
+      </c>
+      <c r="G17" t="s">
+        <v>374</v>
+      </c>
+      <c r="H17" t="s">
+        <v>262</v>
+      </c>
+      <c r="I17" t="s">
+        <v>263</v>
+      </c>
+      <c r="J17" t="s">
+        <v>264</v>
+      </c>
+      <c r="K17" t="s">
+        <v>264</v>
+      </c>
+      <c r="L17" t="s">
+        <v>264</v>
+      </c>
+      <c r="M17" t="s">
+        <v>393</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Olivia", "Perez", LocalDate.of(1952,7, 7),9234568,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>323</v>
+      </c>
+      <c r="B18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>325</v>
+      </c>
+      <c r="F18">
+        <v>28567532</v>
+      </c>
+      <c r="G18" t="s">
+        <v>375</v>
+      </c>
+      <c r="H18" t="s">
+        <v>280</v>
+      </c>
+      <c r="I18" t="s">
+        <v>263</v>
+      </c>
+      <c r="J18" t="s">
+        <v>264</v>
+      </c>
+      <c r="K18" t="s">
+        <v>264</v>
+      </c>
+      <c r="L18" t="s">
+        <v>264</v>
+      </c>
+      <c r="M18" t="s">
+        <v>393</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Andres", "Maldini", LocalDate.of(1981,1, 19),28567532,Gender.MALE, "Banfield", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B19" t="s">
+        <v>327</v>
+      </c>
+      <c r="C19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>300</v>
+      </c>
+      <c r="F19">
+        <v>26123982</v>
+      </c>
+      <c r="G19" t="s">
+        <v>375</v>
+      </c>
+      <c r="H19" t="s">
+        <v>262</v>
+      </c>
+      <c r="I19" t="s">
+        <v>263</v>
+      </c>
+      <c r="J19" t="s">
+        <v>264</v>
+      </c>
+      <c r="K19" t="s">
+        <v>264</v>
+      </c>
+      <c r="L19" t="s">
+        <v>264</v>
+      </c>
+      <c r="M19" t="s">
+        <v>393</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Sebastian", "Titolo", LocalDate.of(1980,7, 3),26123982,Gender.MALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" t="s">
+        <v>328</v>
+      </c>
+      <c r="C20" t="s">
+        <v>329</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>330</v>
+      </c>
+      <c r="F20">
+        <v>37091840</v>
+      </c>
+      <c r="G20" t="s">
+        <v>374</v>
+      </c>
+      <c r="H20" t="s">
+        <v>283</v>
+      </c>
+      <c r="I20" t="s">
+        <v>264</v>
+      </c>
+      <c r="J20" t="s">
+        <v>264</v>
+      </c>
+      <c r="K20" t="s">
+        <v>263</v>
+      </c>
+      <c r="L20" t="s">
+        <v>264</v>
+      </c>
+      <c r="M20" t="s">
+        <v>393</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Camila", "Ensilla", LocalDate.of(1990,10, 2),37091840,Gender.FEMALE, "Lomas", false, false, true, false, false);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" t="s">
+        <v>332</v>
+      </c>
+      <c r="C21" t="s">
+        <v>286</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>322</v>
+      </c>
+      <c r="F21">
+        <v>290911112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>375</v>
+      </c>
+      <c r="H21" t="s">
+        <v>292</v>
+      </c>
+      <c r="I21" t="s">
+        <v>263</v>
+      </c>
+      <c r="J21" t="s">
+        <v>264</v>
+      </c>
+      <c r="K21" t="s">
+        <v>264</v>
+      </c>
+      <c r="L21" t="s">
+        <v>264</v>
+      </c>
+      <c r="M21" t="s">
+        <v>393</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Roberto", "Burgos", LocalDate.of(1982,7, 7),290911112,Gender.MALE, "CABA", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>333</v>
+      </c>
+      <c r="B22" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" t="s">
+        <v>335</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F22">
+        <v>25763201</v>
+      </c>
+      <c r="G22" t="s">
+        <v>375</v>
+      </c>
+      <c r="H22" t="s">
+        <v>292</v>
+      </c>
+      <c r="I22" t="s">
+        <v>263</v>
+      </c>
+      <c r="J22" t="s">
+        <v>263</v>
+      </c>
+      <c r="K22" t="s">
+        <v>264</v>
+      </c>
+      <c r="L22" t="s">
+        <v>264</v>
+      </c>
+      <c r="M22" t="s">
+        <v>393</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Hugo", "Fernandez", LocalDate.of(1977,9, 10),25763201,Gender.MALE, "CABA", true, true, false, false, false);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>336</v>
+      </c>
+      <c r="B23" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" t="s">
+        <v>338</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>339</v>
+      </c>
+      <c r="F23">
+        <v>18888881</v>
+      </c>
+      <c r="G23" t="s">
+        <v>375</v>
+      </c>
+      <c r="H23" t="s">
+        <v>283</v>
+      </c>
+      <c r="I23" t="s">
+        <v>263</v>
+      </c>
+      <c r="J23" t="s">
+        <v>263</v>
+      </c>
+      <c r="K23" t="s">
+        <v>253</v>
+      </c>
+      <c r="L23" t="s">
+        <v>263</v>
+      </c>
+      <c r="M23" t="s">
+        <v>393</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("German", "Castro", LocalDate.of(1967,1, 28),18888881,Gender.MALE, "Lomas", true, true,true, true, false);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>326</v>
+      </c>
+      <c r="B24" t="s">
+        <v>340</v>
+      </c>
+      <c r="C24" t="s">
+        <v>341</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>296</v>
+      </c>
+      <c r="F24">
+        <v>261117625</v>
+      </c>
+      <c r="G24" t="s">
+        <v>375</v>
+      </c>
+      <c r="H24" t="s">
+        <v>292</v>
+      </c>
+      <c r="I24" t="s">
+        <v>263</v>
+      </c>
+      <c r="J24" t="s">
+        <v>264</v>
+      </c>
+      <c r="K24" t="s">
+        <v>264</v>
+      </c>
+      <c r="L24" t="s">
+        <v>264</v>
+      </c>
+      <c r="M24" t="s">
+        <v>393</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Sebastian", "Palmiero", LocalDate.of(1979,9, 10),261117625,Gender.MALE, "CABA", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>342</v>
+      </c>
+      <c r="B25" t="s">
+        <v>343</v>
+      </c>
+      <c r="C25" t="s">
+        <v>344</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>339</v>
+      </c>
+      <c r="F25">
+        <v>33554109</v>
+      </c>
+      <c r="G25" t="s">
+        <v>375</v>
+      </c>
+      <c r="H25" t="s">
+        <v>283</v>
+      </c>
+      <c r="I25" t="s">
+        <v>263</v>
+      </c>
+      <c r="J25" t="s">
+        <v>264</v>
+      </c>
+      <c r="K25" t="s">
+        <v>264</v>
+      </c>
+      <c r="L25" t="s">
+        <v>264</v>
+      </c>
+      <c r="M25" t="s">
+        <v>393</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Gustavo", "Bermudez", LocalDate.of(1986,6, 28),33554109,Gender.MALE, "Lomas", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>345</v>
+      </c>
+      <c r="B26" t="s">
+        <v>346</v>
+      </c>
+      <c r="C26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D26">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>347</v>
+      </c>
+      <c r="F26">
+        <v>31311256</v>
+      </c>
+      <c r="G26" t="s">
+        <v>375</v>
+      </c>
+      <c r="H26" t="s">
+        <v>310</v>
+      </c>
+      <c r="I26" t="s">
+        <v>264</v>
+      </c>
+      <c r="J26" t="s">
+        <v>264</v>
+      </c>
+      <c r="K26" t="s">
+        <v>264</v>
+      </c>
+      <c r="L26" t="s">
+        <v>263</v>
+      </c>
+      <c r="M26" t="s">
+        <v>393</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Anabela", "Lucia", LocalDate.of(1983,8, 12),31311256,Gender.MALE, "Temperley", false, false, false, true, false);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>326</v>
+      </c>
+      <c r="B27" t="s">
+        <v>348</v>
+      </c>
+      <c r="C27" t="s">
+        <v>303</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>347</v>
+      </c>
+      <c r="F27">
+        <v>30137911</v>
+      </c>
+      <c r="G27" t="s">
+        <v>375</v>
+      </c>
+      <c r="H27" t="s">
+        <v>292</v>
+      </c>
+      <c r="I27" t="s">
+        <v>263</v>
+      </c>
+      <c r="J27" t="s">
+        <v>264</v>
+      </c>
+      <c r="K27" t="s">
+        <v>264</v>
+      </c>
+      <c r="L27" t="s">
+        <v>264</v>
+      </c>
+      <c r="M27" t="s">
+        <v>393</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Sebastian", "Saccani", LocalDate.of(1985,12, 12),30137911,Gender.MALE, "CABA", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>349</v>
+      </c>
+      <c r="B28" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" t="s">
+        <v>350</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>351</v>
+      </c>
+      <c r="F28">
+        <v>36009272</v>
+      </c>
+      <c r="G28" t="s">
+        <v>374</v>
+      </c>
+      <c r="H28" t="s">
+        <v>262</v>
+      </c>
+      <c r="I28" t="s">
+        <v>263</v>
+      </c>
+      <c r="J28" t="s">
+        <v>264</v>
+      </c>
+      <c r="K28" t="s">
+        <v>264</v>
+      </c>
+      <c r="L28" t="s">
+        <v>264</v>
+      </c>
+      <c r="M28" t="s">
+        <v>393</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Natalia", "Saccani", LocalDate.of(1989,6, 13),36009272,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>349</v>
+      </c>
+      <c r="B29" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" t="s">
+        <v>329</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>351</v>
+      </c>
+      <c r="F29">
+        <v>40192827</v>
+      </c>
+      <c r="G29" t="s">
+        <v>375</v>
+      </c>
+      <c r="H29" t="s">
+        <v>262</v>
+      </c>
+      <c r="I29" t="s">
+        <v>264</v>
+      </c>
+      <c r="J29" t="s">
+        <v>264</v>
+      </c>
+      <c r="K29" t="s">
+        <v>264</v>
+      </c>
+      <c r="L29" t="s">
+        <v>263</v>
+      </c>
+      <c r="M29" t="s">
+        <v>393</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Natalia", "Damele", LocalDate.of(1990,1, 13),40192827,Gender.MALE, "Lanus", false, false, false, true, false);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>353</v>
+      </c>
+      <c r="B30" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" t="s">
+        <v>355</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>325</v>
+      </c>
+      <c r="F30">
+        <v>45029126</v>
+      </c>
+      <c r="G30" t="s">
+        <v>375</v>
+      </c>
+      <c r="H30" t="s">
+        <v>292</v>
+      </c>
+      <c r="I30" t="s">
+        <v>263</v>
+      </c>
+      <c r="J30" t="s">
+        <v>264</v>
+      </c>
+      <c r="K30" t="s">
+        <v>264</v>
+      </c>
+      <c r="L30" t="s">
+        <v>264</v>
+      </c>
+      <c r="M30" t="s">
+        <v>393</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Eliana", "Matera", LocalDate.of(1994,11, 19),45029126,Gender.MALE, "CABA", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>356</v>
+      </c>
+      <c r="B31" t="s">
+        <v>357</v>
+      </c>
+      <c r="C31" t="s">
+        <v>344</v>
+      </c>
+      <c r="D31">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>358</v>
+      </c>
+      <c r="F31">
+        <v>33245927</v>
+      </c>
+      <c r="G31" t="s">
+        <v>374</v>
+      </c>
+      <c r="H31" t="s">
+        <v>283</v>
+      </c>
+      <c r="I31" t="s">
+        <v>263</v>
+      </c>
+      <c r="J31" t="s">
+        <v>264</v>
+      </c>
+      <c r="K31" t="s">
+        <v>264</v>
+      </c>
+      <c r="L31" t="s">
+        <v>264</v>
+      </c>
+      <c r="M31" t="s">
+        <v>393</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Florencia", "Persiani", LocalDate.of(1986,9, 20),33245927,Gender.FEMALE, "Lomas", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>356</v>
+      </c>
+      <c r="B32" t="s">
+        <v>359</v>
+      </c>
+      <c r="C32" t="s">
+        <v>360</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>347</v>
+      </c>
+      <c r="F32">
+        <v>37726189</v>
+      </c>
+      <c r="G32" t="s">
+        <v>374</v>
+      </c>
+      <c r="H32" t="s">
+        <v>262</v>
+      </c>
+      <c r="I32" t="s">
+        <v>264</v>
+      </c>
+      <c r="J32" t="s">
+        <v>264</v>
+      </c>
+      <c r="K32" t="s">
+        <v>264</v>
+      </c>
+      <c r="L32" t="s">
+        <v>263</v>
+      </c>
+      <c r="M32" t="s">
+        <v>393</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Florencia", "De Lucca", LocalDate.of(1991,5, 12),37726189,Gender.FEMALE, "Lanus", false, false, false, true, false);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>361</v>
+      </c>
+      <c r="B33" t="s">
+        <v>362</v>
+      </c>
+      <c r="C33" t="s">
+        <v>363</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>364</v>
+      </c>
+      <c r="F33">
+        <v>13916645</v>
+      </c>
+      <c r="G33" t="s">
+        <v>375</v>
+      </c>
+      <c r="H33" t="s">
+        <v>292</v>
+      </c>
+      <c r="I33" t="s">
+        <v>263</v>
+      </c>
+      <c r="J33" t="s">
+        <v>264</v>
+      </c>
+      <c r="K33" t="s">
+        <v>264</v>
+      </c>
+      <c r="L33" t="s">
+        <v>264</v>
+      </c>
+      <c r="M33" t="s">
+        <v>393</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Norma", "Ponce", LocalDate.of(1968,5, 4),13916645,Gender.MALE, "CABA", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>356</v>
+      </c>
+      <c r="B34" t="s">
+        <v>365</v>
+      </c>
+      <c r="C34" t="s">
+        <v>366</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>351</v>
+      </c>
+      <c r="F34">
+        <v>46782722</v>
+      </c>
+      <c r="G34" t="s">
+        <v>374</v>
+      </c>
+      <c r="H34" t="s">
+        <v>262</v>
+      </c>
+      <c r="I34" t="s">
+        <v>263</v>
+      </c>
+      <c r="J34" t="s">
+        <v>264</v>
+      </c>
+      <c r="K34" t="s">
+        <v>264</v>
+      </c>
+      <c r="L34" t="s">
+        <v>264</v>
+      </c>
+      <c r="M34" t="s">
+        <v>393</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Florencia", "Salamanca", LocalDate.of(1995,6, 13),46782722,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>367</v>
+      </c>
+      <c r="B35" t="s">
+        <v>368</v>
+      </c>
+      <c r="C35" t="s">
+        <v>286</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>369</v>
+      </c>
+      <c r="F35">
+        <v>29786687</v>
+      </c>
+      <c r="G35" t="s">
+        <v>374</v>
+      </c>
+      <c r="H35" t="s">
+        <v>262</v>
+      </c>
+      <c r="I35" t="s">
+        <v>263</v>
+      </c>
+      <c r="J35" t="s">
+        <v>264</v>
+      </c>
+      <c r="K35" t="s">
+        <v>264</v>
+      </c>
+      <c r="L35" t="s">
+        <v>264</v>
+      </c>
+      <c r="M35" t="s">
+        <v>393</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Vanesa", "Apodaca", LocalDate.of(1982,5, 14),29786687,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>370</v>
+      </c>
+      <c r="B36" t="s">
+        <v>308</v>
+      </c>
+      <c r="C36" t="s">
+        <v>371</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>318</v>
+      </c>
+      <c r="F36">
+        <v>35781115</v>
+      </c>
+      <c r="G36" t="s">
+        <v>375</v>
+      </c>
+      <c r="H36" t="s">
+        <v>262</v>
+      </c>
+      <c r="I36" t="s">
+        <v>263</v>
+      </c>
+      <c r="J36" t="s">
+        <v>264</v>
+      </c>
+      <c r="K36" t="s">
+        <v>264</v>
+      </c>
+      <c r="L36" t="s">
+        <v>264</v>
+      </c>
+      <c r="M36" t="s">
+        <v>393</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Gabriel", "Perez", LocalDate.of(1988,3, 27),35781115,Gender.MALE, "Lanus", true, false, false, false, false);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>372</v>
+      </c>
+      <c r="B37" t="s">
+        <v>373</v>
+      </c>
+      <c r="C37" t="s">
+        <v>315</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>296</v>
+      </c>
+      <c r="F37">
+        <v>31766985</v>
+      </c>
+      <c r="G37" t="s">
+        <v>375</v>
+      </c>
+      <c r="H37" t="s">
+        <v>262</v>
+      </c>
+      <c r="I37" t="s">
+        <v>263</v>
+      </c>
+      <c r="J37" t="s">
+        <v>264</v>
+      </c>
+      <c r="K37" t="s">
+        <v>252</v>
+      </c>
+      <c r="L37" t="s">
+        <v>264</v>
+      </c>
+      <c r="M37" t="s">
+        <v>393</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="0"/>
+        <v>tempPatient = new Patient("Gonzalo", "Marcec", LocalDate.of(1984,7, 10),31766985,Gender.MALE, "Lanus", true, false,false, false, false);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F947F389-137E-47A9-B6AD-45D161DF4B81}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
@@ -2651,7 +4356,7 @@
     <col min="15" max="15" width="1.47265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.83984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="1.47265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.47265625" style="79" customWidth="1"/>
+    <col min="18" max="18" width="1.47265625" style="54" customWidth="1"/>
     <col min="19" max="19" width="8.20703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.15625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="76.3671875" bestFit="1" customWidth="1"/>
@@ -5154,7 +6859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E75605B5-9BA1-4DBA-9958-FDD7A98EA7A9}">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -5953,11 +7658,98 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DB8F3D-8B49-45A6-A91B-89335D16DD2B}">
+  <dimension ref="C1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.41796875" customWidth="1"/>
+    <col min="2" max="2" width="4.83984375" customWidth="1"/>
+    <col min="3" max="3" width="57.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.26171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C1" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="61"/>
+    </row>
+    <row r="2" spans="3:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C2" s="58" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+    </row>
+    <row r="3" spans="3:6" s="1" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C3" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C4" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="6" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C6" s="60" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6" s="61"/>
+    </row>
+    <row r="7" spans="3:6" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C7" s="58" t="s">
+        <v>401</v>
+      </c>
+      <c r="D7" s="59"/>
+    </row>
+    <row r="8" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C8" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C9" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>398</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F436EEA-E025-4904-8C51-7AE523CEFF50}">
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5969,16 +7761,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="54"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="2" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C2" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
     </row>
@@ -5999,20 +7791,20 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="67"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
@@ -6041,18 +7833,18 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="67"/>
+      <c r="D11" s="63"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="D12" s="61"/>
+      <c r="D12" s="67"/>
     </row>
     <row r="13" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C13" s="34" t="s">
@@ -6079,18 +7871,18 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="62"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="66" t="s">
         <v>226</v>
       </c>
-      <c r="D17" s="61"/>
+      <c r="D17" s="67"/>
     </row>
     <row r="18" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C18" s="34" t="s">
@@ -6115,16 +7907,16 @@
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="62"/>
+      <c r="D21" s="68"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="69" t="s">
         <v>227</v>
       </c>
-      <c r="D22" s="64"/>
+      <c r="D22" s="70"/>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
     </row>
@@ -6153,20 +7945,20 @@
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="68" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
     </row>
     <row r="27" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="66" t="s">
         <v>235</v>
       </c>
-      <c r="D27" s="61"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
@@ -6193,10 +7985,10 @@
     <row r="31" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="53" t="s">
+      <c r="C31" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="54"/>
+      <c r="D31" s="61"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
@@ -6204,7 +7996,7 @@
       <c r="C32" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="59"/>
+      <c r="D32" s="74"/>
     </row>
     <row r="33" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C33" s="34" t="s">
@@ -6226,16 +8018,16 @@
     </row>
     <row r="35" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="36" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C36" s="53" t="s">
+      <c r="C36" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="D36" s="54"/>
+      <c r="D36" s="61"/>
     </row>
     <row r="37" spans="3:6" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="71" t="s">
         <v>241</v>
       </c>
-      <c r="D37" s="56"/>
+      <c r="D37" s="72"/>
     </row>
     <row r="38" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C38" s="34" t="s">
@@ -6255,16 +8047,16 @@
     </row>
     <row r="40" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="41" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C41" s="53" t="s">
+      <c r="C41" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="D41" s="57"/>
+      <c r="D41" s="73"/>
     </row>
     <row r="42" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C42" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="D42" s="59"/>
+      <c r="D42" s="74"/>
     </row>
     <row r="43" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C43" s="34" t="s">
@@ -6284,17 +8076,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C41:D41"/>
@@ -6302,18 +8083,29 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D328F27E-EB15-4084-9540-33BF77EBB9A1}">
   <dimension ref="A1:AR43"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8274,22 +10066,22 @@
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="76" t="s">
+      <c r="A26" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="77">
+      <c r="B26" s="52">
         <v>0.61458333333333404</v>
       </c>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="77">
+      <c r="D26" s="52">
         <v>0.61458333333333404</v>
       </c>
-      <c r="E26" s="77">
+      <c r="E26" s="52">
         <v>0.624999999999999</v>
       </c>
-      <c r="F26" s="78">
+      <c r="F26" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -10211,43 +12003,43 @@
       </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="75" t="s">
         <v>248</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="70"/>
-      <c r="M41" s="70"/>
-      <c r="N41" s="70"/>
-      <c r="O41" s="70"/>
-      <c r="P41" s="70"/>
-      <c r="Q41" s="70"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="75"/>
+      <c r="M41" s="75"/>
+      <c r="N41" s="75"/>
+      <c r="O41" s="75"/>
+      <c r="P41" s="75"/>
+      <c r="Q41" s="75"/>
     </row>
     <row r="42" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="75" t="s">
         <v>249</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="70"/>
-      <c r="M42" s="70"/>
-      <c r="N42" s="70"/>
-      <c r="O42" s="70"/>
-      <c r="P42" s="70"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="75"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="75"/>
+      <c r="M42" s="75"/>
+      <c r="N42" s="75"/>
+      <c r="O42" s="75"/>
+      <c r="P42" s="75"/>
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="44" t="s">
@@ -10264,7 +12056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AAC928-D5F2-4412-8D8F-A754DC5B9F83}">
   <dimension ref="A1:AT38"/>
   <sheetViews>
@@ -10509,7 +12301,7 @@
         <v>0.3888888888888889</v>
       </c>
       <c r="E4" s="6">
-        <f t="shared" ref="E4:E38" si="1">D4+F4</f>
+        <f t="shared" ref="E4:E31" si="1">D4+F4</f>
         <v>0.39930555555555558</v>
       </c>
       <c r="F4" s="23">
@@ -10517,7 +12309,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="G4" s="17">
-        <f t="shared" ref="G4:G38" si="2">MINUTE(E4-(B4+$G$1))</f>
+        <f t="shared" ref="G4:G31" si="2">MINUTE(E4-(B4+$G$1))</f>
         <v>5</v>
       </c>
       <c r="H4" s="17" t="str">
@@ -13593,18 +15385,18 @@
       </c>
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="77">
+      <c r="B34" s="52">
         <v>0.69791666666666696</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C34" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="80">
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="55">
         <f t="shared" si="25"/>
         <v>1.0416666666666666E-2</v>
       </c>
@@ -13742,11 +15534,11 @@
         <f t="shared" si="36"/>
         <v>0.72916666666666696</v>
       </c>
-      <c r="AO34" s="77">
+      <c r="AO34" s="52">
         <f t="shared" si="38"/>
         <v>0.72916666666666696</v>
       </c>
-      <c r="AP34" s="77">
+      <c r="AP34" s="52">
         <f>$B34+TIME(0,$G$33,0)</f>
         <v>0.72916666666666696</v>
       </c>
@@ -14433,11 +16225,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649E4E89-40C2-4DD8-B2B1-05F39BEB42A4}">
   <dimension ref="A1:AS38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:E34"/>
     </sheetView>
   </sheetViews>
@@ -17608,19 +19400,19 @@
       </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="77">
+      <c r="B34" s="52">
         <v>0.69791666666666696</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C34" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="D34" s="77">
+      <c r="D34" s="52">
         <v>0.69791666666666696</v>
       </c>
-      <c r="E34" s="77">
+      <c r="E34" s="52">
         <v>0.70833333333333304</v>
       </c>
       <c r="F34" s="17">
@@ -18453,7 +20245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93B131D-B47B-4504-8546-4C6786F6BED8}">
   <dimension ref="A1:AO38"/>
   <sheetViews>
@@ -21915,7 +23707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5110DC-726D-4DC0-AC14-F370793D4F4C}">
   <dimension ref="A1:AW51"/>
   <sheetViews>
@@ -29640,28 +31432,28 @@
       </c>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="71" t="s">
+      <c r="A48" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="71"/>
+      <c r="B48" s="76"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="72" t="s">
+      <c r="A49" s="77" t="s">
         <v>189</v>
       </c>
-      <c r="B49" s="72"/>
+      <c r="B49" s="77"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="73" t="s">
+      <c r="A50" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="B50" s="74"/>
+      <c r="B50" s="79"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="75" t="s">
+      <c r="A51" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="B51" s="75"/>
+      <c r="B51" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -29675,7 +31467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70C75B3-17FC-455C-A761-FE2EA48DEA2D}">
   <dimension ref="A1:AP46"/>
   <sheetViews>
@@ -29683,7 +31475,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -35578,32 +37370,32 @@
       </c>
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="71" t="s">
+      <c r="A43" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="B43" s="71"/>
+      <c r="B43" s="76"/>
     </row>
     <row r="44" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="72" t="s">
+      <c r="A44" s="77" t="s">
         <v>189</v>
       </c>
-      <c r="B44" s="72"/>
+      <c r="B44" s="77"/>
       <c r="G44" s="6">
         <f>E10-(B10+$G$1)</f>
         <v>3.4722222222219878E-3</v>
       </c>
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="73" t="s">
+      <c r="A45" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="B45" s="74"/>
+      <c r="B45" s="79"/>
     </row>
     <row r="46" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="75" t="s">
+      <c r="A46" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="B46" s="75"/>
+      <c r="B46" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -35617,1699 +37409,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABED78B2-C549-4968-8087-F00418B9D012}">
-  <dimension ref="A1:O37"/>
-  <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="31.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.62890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.05078125" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="146.05078125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H1" t="s">
-        <v>273</v>
-      </c>
-      <c r="I1" t="s">
-        <v>274</v>
-      </c>
-      <c r="J1" t="s">
-        <v>274</v>
-      </c>
-      <c r="K1" t="s">
-        <v>274</v>
-      </c>
-      <c r="L1" t="s">
-        <v>274</v>
-      </c>
-      <c r="M1" t="s">
-        <v>275</v>
-      </c>
-      <c r="O1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F2">
-        <v>10664879</v>
-      </c>
-      <c r="G2" t="s">
-        <v>375</v>
-      </c>
-      <c r="H2" t="s">
-        <v>262</v>
-      </c>
-      <c r="I2" t="s">
-        <v>264</v>
-      </c>
-      <c r="J2" t="s">
-        <v>263</v>
-      </c>
-      <c r="K2" t="s">
-        <v>264</v>
-      </c>
-      <c r="L2" t="s">
-        <v>264</v>
-      </c>
-      <c r="M2" t="s">
-        <v>393</v>
-      </c>
-      <c r="O2" t="str">
-        <f>_xlfn.TEXTJOIN(",",,A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,)</f>
-        <v>tempPatient = new Patient("Julio", "Arias", LocalDate.of(1953,1, 17),10664879,Gender.MALE, "Lanus", false, true, false, false, false);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C3" t="s">
-        <v>260</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F3">
-        <v>9215788</v>
-      </c>
-      <c r="G3" t="s">
-        <v>374</v>
-      </c>
-      <c r="H3" t="s">
-        <v>262</v>
-      </c>
-      <c r="I3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J3" t="s">
-        <v>264</v>
-      </c>
-      <c r="K3" t="s">
-        <v>264</v>
-      </c>
-      <c r="L3" t="s">
-        <v>264</v>
-      </c>
-      <c r="M3" t="s">
-        <v>393</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O37" si="0">_xlfn.TEXTJOIN(",",,A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,)</f>
-        <v>tempPatient = new Patient("Beatriz", "Leguizamon", LocalDate.of(1955,6, 25),9215788,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>279</v>
-      </c>
-      <c r="F4">
-        <v>30127532</v>
-      </c>
-      <c r="G4" t="s">
-        <v>375</v>
-      </c>
-      <c r="H4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I4" t="s">
-        <v>263</v>
-      </c>
-      <c r="J4" t="s">
-        <v>264</v>
-      </c>
-      <c r="K4" t="s">
-        <v>264</v>
-      </c>
-      <c r="L4" t="s">
-        <v>264</v>
-      </c>
-      <c r="M4" t="s">
-        <v>393</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Cristian", "Vallarino", LocalDate.of(1983,2, 22),30127532,Gender.MALE, "Banfield", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B5" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" t="s">
-        <v>282</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F5">
-        <v>26742442</v>
-      </c>
-      <c r="G5" t="s">
-        <v>374</v>
-      </c>
-      <c r="H5" t="s">
-        <v>283</v>
-      </c>
-      <c r="I5" t="s">
-        <v>263</v>
-      </c>
-      <c r="J5" t="s">
-        <v>264</v>
-      </c>
-      <c r="K5" t="s">
-        <v>264</v>
-      </c>
-      <c r="L5" t="s">
-        <v>264</v>
-      </c>
-      <c r="M5" t="s">
-        <v>393</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Victoria", "Arias", LocalDate.of(1980,1, 25),26742442,Gender.FEMALE, "Lomas", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B6" t="s">
-        <v>285</v>
-      </c>
-      <c r="C6" t="s">
-        <v>286</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>287</v>
-      </c>
-      <c r="F6">
-        <v>30333982</v>
-      </c>
-      <c r="G6" t="s">
-        <v>374</v>
-      </c>
-      <c r="H6" t="s">
-        <v>283</v>
-      </c>
-      <c r="I6" t="s">
-        <v>264</v>
-      </c>
-      <c r="J6" t="s">
-        <v>264</v>
-      </c>
-      <c r="K6" t="s">
-        <v>263</v>
-      </c>
-      <c r="L6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M6" t="s">
-        <v>393</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Camila", "Garcia", LocalDate.of(1982,7, 9),30333982,Gender.FEMALE, "Lomas", false, false, true, false, false);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>288</v>
-      </c>
-      <c r="B7" t="s">
-        <v>289</v>
-      </c>
-      <c r="C7" t="s">
-        <v>290</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F7">
-        <v>28447445</v>
-      </c>
-      <c r="G7" t="s">
-        <v>374</v>
-      </c>
-      <c r="H7" t="s">
-        <v>292</v>
-      </c>
-      <c r="I7" t="s">
-        <v>263</v>
-      </c>
-      <c r="J7" t="s">
-        <v>264</v>
-      </c>
-      <c r="K7" t="s">
-        <v>264</v>
-      </c>
-      <c r="L7" t="s">
-        <v>264</v>
-      </c>
-      <c r="M7" t="s">
-        <v>393</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Gabriela", "Suarez", LocalDate.of(1981,11, 11),28447445,Gender.FEMALE, "CABA", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8" t="s">
-        <v>295</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F8">
-        <v>25725839</v>
-      </c>
-      <c r="G8" t="s">
-        <v>375</v>
-      </c>
-      <c r="H8" t="s">
-        <v>292</v>
-      </c>
-      <c r="I8" t="s">
-        <v>263</v>
-      </c>
-      <c r="J8" t="s">
-        <v>263</v>
-      </c>
-      <c r="K8" t="s">
-        <v>264</v>
-      </c>
-      <c r="L8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M8" t="s">
-        <v>393</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Francisco", "De Marco", LocalDate.of(1978,9, 10),25725839,Gender.MALE, "CABA", true, true, false, false, false);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>297</v>
-      </c>
-      <c r="B9" t="s">
-        <v>298</v>
-      </c>
-      <c r="C9" t="s">
-        <v>299</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>300</v>
-      </c>
-      <c r="F9">
-        <v>20876091</v>
-      </c>
-      <c r="G9" t="s">
-        <v>375</v>
-      </c>
-      <c r="H9" t="s">
-        <v>283</v>
-      </c>
-      <c r="I9" t="s">
-        <v>263</v>
-      </c>
-      <c r="J9" t="s">
-        <v>263</v>
-      </c>
-      <c r="K9" t="s">
-        <v>263</v>
-      </c>
-      <c r="L9" t="s">
-        <v>263</v>
-      </c>
-      <c r="M9" t="s">
-        <v>393</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Emilio", "Dissi", LocalDate.of(1970,3, 3),20876091,Gender.MALE, "Lomas", true, true, true, true, false);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>301</v>
-      </c>
-      <c r="B10" t="s">
-        <v>302</v>
-      </c>
-      <c r="C10" t="s">
-        <v>303</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>304</v>
-      </c>
-      <c r="F10">
-        <v>33445775</v>
-      </c>
-      <c r="G10" t="s">
-        <v>374</v>
-      </c>
-      <c r="H10" t="s">
-        <v>262</v>
-      </c>
-      <c r="I10" t="s">
-        <v>263</v>
-      </c>
-      <c r="J10" t="s">
-        <v>264</v>
-      </c>
-      <c r="K10" t="s">
-        <v>264</v>
-      </c>
-      <c r="L10" t="s">
-        <v>264</v>
-      </c>
-      <c r="M10" t="s">
-        <v>393</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Iris", "De Ojo", LocalDate.of(1985,9, 1),33445775,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11" t="s">
-        <v>306</v>
-      </c>
-      <c r="C11" t="s">
-        <v>290</v>
-      </c>
-      <c r="D11">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>291</v>
-      </c>
-      <c r="F11">
-        <v>22987456</v>
-      </c>
-      <c r="G11" t="s">
-        <v>375</v>
-      </c>
-      <c r="H11" t="s">
-        <v>283</v>
-      </c>
-      <c r="I11" t="s">
-        <v>263</v>
-      </c>
-      <c r="J11" t="s">
-        <v>264</v>
-      </c>
-      <c r="K11" t="s">
-        <v>264</v>
-      </c>
-      <c r="L11" t="s">
-        <v>264</v>
-      </c>
-      <c r="M11" t="s">
-        <v>393</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Luciano", "Lunga", LocalDate.of(1981,11, 11),22987456,Gender.MALE, "Lomas", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>307</v>
-      </c>
-      <c r="B12" t="s">
-        <v>308</v>
-      </c>
-      <c r="C12" t="s">
-        <v>286</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>309</v>
-      </c>
-      <c r="F12">
-        <v>29851753</v>
-      </c>
-      <c r="G12" t="s">
-        <v>375</v>
-      </c>
-      <c r="H12" t="s">
-        <v>310</v>
-      </c>
-      <c r="I12" t="s">
-        <v>264</v>
-      </c>
-      <c r="J12" t="s">
-        <v>264</v>
-      </c>
-      <c r="K12" t="s">
-        <v>264</v>
-      </c>
-      <c r="L12" t="s">
-        <v>263</v>
-      </c>
-      <c r="M12" t="s">
-        <v>393</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Alejo", "Perez", LocalDate.of(1982,2, 15),29851753,Gender.MALE, "Temperley", false, false, false, true, false);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>311</v>
-      </c>
-      <c r="B13" t="s">
-        <v>308</v>
-      </c>
-      <c r="C13" t="s">
-        <v>282</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>261</v>
-      </c>
-      <c r="F13">
-        <v>29356543</v>
-      </c>
-      <c r="G13" t="s">
-        <v>374</v>
-      </c>
-      <c r="H13" t="s">
-        <v>262</v>
-      </c>
-      <c r="I13" t="s">
-        <v>264</v>
-      </c>
-      <c r="J13" t="s">
-        <v>263</v>
-      </c>
-      <c r="K13" t="s">
-        <v>264</v>
-      </c>
-      <c r="L13" t="s">
-        <v>264</v>
-      </c>
-      <c r="M13" t="s">
-        <v>393</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Paula", "Perez", LocalDate.of(1980,2, 25),29356543,Gender.FEMALE, "Lanus", false, true, false, false, false);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>265</v>
-      </c>
-      <c r="B14" t="s">
-        <v>312</v>
-      </c>
-      <c r="C14" t="s">
-        <v>260</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>309</v>
-      </c>
-      <c r="F14">
-        <v>12615229</v>
-      </c>
-      <c r="G14" t="s">
-        <v>375</v>
-      </c>
-      <c r="H14" t="s">
-        <v>262</v>
-      </c>
-      <c r="I14" t="s">
-        <v>264</v>
-      </c>
-      <c r="J14" t="s">
-        <v>264</v>
-      </c>
-      <c r="K14" t="s">
-        <v>264</v>
-      </c>
-      <c r="L14" t="s">
-        <v>264</v>
-      </c>
-      <c r="M14" t="s">
-        <v>393</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Julio", "Sanchez", LocalDate.of(1955,5, 15),12615229,Gender.MALE, "Lanus", false, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>313</v>
-      </c>
-      <c r="B15" t="s">
-        <v>314</v>
-      </c>
-      <c r="C15" t="s">
-        <v>315</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>309</v>
-      </c>
-      <c r="F15">
-        <v>33153323</v>
-      </c>
-      <c r="G15" t="s">
-        <v>374</v>
-      </c>
-      <c r="H15" t="s">
-        <v>262</v>
-      </c>
-      <c r="I15" t="s">
-        <v>264</v>
-      </c>
-      <c r="J15" t="s">
-        <v>264</v>
-      </c>
-      <c r="K15" t="s">
-        <v>264</v>
-      </c>
-      <c r="L15" t="s">
-        <v>264</v>
-      </c>
-      <c r="M15" t="s">
-        <v>393</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Laura", "Bonilla", LocalDate.of(1984,5, 15),33153323,Gender.FEMALE, "Lanus", false, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>316</v>
-      </c>
-      <c r="B16" t="s">
-        <v>317</v>
-      </c>
-      <c r="C16" t="s">
-        <v>286</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>318</v>
-      </c>
-      <c r="F16">
-        <v>29445256</v>
-      </c>
-      <c r="G16" t="s">
-        <v>374</v>
-      </c>
-      <c r="H16" t="s">
-        <v>319</v>
-      </c>
-      <c r="I16" t="s">
-        <v>263</v>
-      </c>
-      <c r="J16" t="s">
-        <v>263</v>
-      </c>
-      <c r="K16" t="s">
-        <v>264</v>
-      </c>
-      <c r="L16" t="s">
-        <v>264</v>
-      </c>
-      <c r="M16" t="s">
-        <v>393</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Andrea", "Gonzales", LocalDate.of(1982,2, 27),29445256,Gender.FEMALE, "Temperlay", true, true, false, false, false);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>320</v>
-      </c>
-      <c r="B17" t="s">
-        <v>308</v>
-      </c>
-      <c r="C17" t="s">
-        <v>321</v>
-      </c>
-      <c r="D17">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>322</v>
-      </c>
-      <c r="F17">
-        <v>9234568</v>
-      </c>
-      <c r="G17" t="s">
-        <v>374</v>
-      </c>
-      <c r="H17" t="s">
-        <v>262</v>
-      </c>
-      <c r="I17" t="s">
-        <v>263</v>
-      </c>
-      <c r="J17" t="s">
-        <v>264</v>
-      </c>
-      <c r="K17" t="s">
-        <v>264</v>
-      </c>
-      <c r="L17" t="s">
-        <v>264</v>
-      </c>
-      <c r="M17" t="s">
-        <v>393</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Olivia", "Perez", LocalDate.of(1952,7, 7),9234568,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>323</v>
-      </c>
-      <c r="B18" t="s">
-        <v>324</v>
-      </c>
-      <c r="C18" t="s">
-        <v>290</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>325</v>
-      </c>
-      <c r="F18">
-        <v>28567532</v>
-      </c>
-      <c r="G18" t="s">
-        <v>375</v>
-      </c>
-      <c r="H18" t="s">
-        <v>280</v>
-      </c>
-      <c r="I18" t="s">
-        <v>263</v>
-      </c>
-      <c r="J18" t="s">
-        <v>264</v>
-      </c>
-      <c r="K18" t="s">
-        <v>264</v>
-      </c>
-      <c r="L18" t="s">
-        <v>264</v>
-      </c>
-      <c r="M18" t="s">
-        <v>393</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Andres", "Maldini", LocalDate.of(1981,1, 19),28567532,Gender.MALE, "Banfield", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>326</v>
-      </c>
-      <c r="B19" t="s">
-        <v>327</v>
-      </c>
-      <c r="C19" t="s">
-        <v>282</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>300</v>
-      </c>
-      <c r="F19">
-        <v>26123982</v>
-      </c>
-      <c r="G19" t="s">
-        <v>375</v>
-      </c>
-      <c r="H19" t="s">
-        <v>262</v>
-      </c>
-      <c r="I19" t="s">
-        <v>263</v>
-      </c>
-      <c r="J19" t="s">
-        <v>264</v>
-      </c>
-      <c r="K19" t="s">
-        <v>264</v>
-      </c>
-      <c r="L19" t="s">
-        <v>264</v>
-      </c>
-      <c r="M19" t="s">
-        <v>393</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Sebastian", "Titolo", LocalDate.of(1980,7, 3),26123982,Gender.MALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>284</v>
-      </c>
-      <c r="B20" t="s">
-        <v>328</v>
-      </c>
-      <c r="C20" t="s">
-        <v>329</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>330</v>
-      </c>
-      <c r="F20">
-        <v>37091840</v>
-      </c>
-      <c r="G20" t="s">
-        <v>374</v>
-      </c>
-      <c r="H20" t="s">
-        <v>283</v>
-      </c>
-      <c r="I20" t="s">
-        <v>264</v>
-      </c>
-      <c r="J20" t="s">
-        <v>264</v>
-      </c>
-      <c r="K20" t="s">
-        <v>263</v>
-      </c>
-      <c r="L20" t="s">
-        <v>264</v>
-      </c>
-      <c r="M20" t="s">
-        <v>393</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Camila", "Ensilla", LocalDate.of(1990,10, 2),37091840,Gender.FEMALE, "Lomas", false, false, true, false, false);</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>331</v>
-      </c>
-      <c r="B21" t="s">
-        <v>332</v>
-      </c>
-      <c r="C21" t="s">
-        <v>286</v>
-      </c>
-      <c r="D21">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>322</v>
-      </c>
-      <c r="F21">
-        <v>290911112</v>
-      </c>
-      <c r="G21" t="s">
-        <v>375</v>
-      </c>
-      <c r="H21" t="s">
-        <v>292</v>
-      </c>
-      <c r="I21" t="s">
-        <v>263</v>
-      </c>
-      <c r="J21" t="s">
-        <v>264</v>
-      </c>
-      <c r="K21" t="s">
-        <v>264</v>
-      </c>
-      <c r="L21" t="s">
-        <v>264</v>
-      </c>
-      <c r="M21" t="s">
-        <v>393</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Roberto", "Burgos", LocalDate.of(1982,7, 7),290911112,Gender.MALE, "CABA", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>333</v>
-      </c>
-      <c r="B22" t="s">
-        <v>334</v>
-      </c>
-      <c r="C22" t="s">
-        <v>335</v>
-      </c>
-      <c r="D22">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>296</v>
-      </c>
-      <c r="F22">
-        <v>25763201</v>
-      </c>
-      <c r="G22" t="s">
-        <v>375</v>
-      </c>
-      <c r="H22" t="s">
-        <v>292</v>
-      </c>
-      <c r="I22" t="s">
-        <v>263</v>
-      </c>
-      <c r="J22" t="s">
-        <v>263</v>
-      </c>
-      <c r="K22" t="s">
-        <v>264</v>
-      </c>
-      <c r="L22" t="s">
-        <v>264</v>
-      </c>
-      <c r="M22" t="s">
-        <v>393</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Hugo", "Fernandez", LocalDate.of(1977,9, 10),25763201,Gender.MALE, "CABA", true, true, false, false, false);</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>336</v>
-      </c>
-      <c r="B23" t="s">
-        <v>337</v>
-      </c>
-      <c r="C23" t="s">
-        <v>338</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>339</v>
-      </c>
-      <c r="F23">
-        <v>18888881</v>
-      </c>
-      <c r="G23" t="s">
-        <v>375</v>
-      </c>
-      <c r="H23" t="s">
-        <v>283</v>
-      </c>
-      <c r="I23" t="s">
-        <v>263</v>
-      </c>
-      <c r="J23" t="s">
-        <v>263</v>
-      </c>
-      <c r="K23" t="s">
-        <v>253</v>
-      </c>
-      <c r="L23" t="s">
-        <v>263</v>
-      </c>
-      <c r="M23" t="s">
-        <v>393</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("German", "Castro", LocalDate.of(1967,1, 28),18888881,Gender.MALE, "Lomas", true, true,true, true, false);</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>326</v>
-      </c>
-      <c r="B24" t="s">
-        <v>340</v>
-      </c>
-      <c r="C24" t="s">
-        <v>341</v>
-      </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>296</v>
-      </c>
-      <c r="F24">
-        <v>261117625</v>
-      </c>
-      <c r="G24" t="s">
-        <v>375</v>
-      </c>
-      <c r="H24" t="s">
-        <v>292</v>
-      </c>
-      <c r="I24" t="s">
-        <v>263</v>
-      </c>
-      <c r="J24" t="s">
-        <v>264</v>
-      </c>
-      <c r="K24" t="s">
-        <v>264</v>
-      </c>
-      <c r="L24" t="s">
-        <v>264</v>
-      </c>
-      <c r="M24" t="s">
-        <v>393</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Sebastian", "Palmiero", LocalDate.of(1979,9, 10),261117625,Gender.MALE, "CABA", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>342</v>
-      </c>
-      <c r="B25" t="s">
-        <v>343</v>
-      </c>
-      <c r="C25" t="s">
-        <v>344</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>339</v>
-      </c>
-      <c r="F25">
-        <v>33554109</v>
-      </c>
-      <c r="G25" t="s">
-        <v>375</v>
-      </c>
-      <c r="H25" t="s">
-        <v>283</v>
-      </c>
-      <c r="I25" t="s">
-        <v>263</v>
-      </c>
-      <c r="J25" t="s">
-        <v>264</v>
-      </c>
-      <c r="K25" t="s">
-        <v>264</v>
-      </c>
-      <c r="L25" t="s">
-        <v>264</v>
-      </c>
-      <c r="M25" t="s">
-        <v>393</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Gustavo", "Bermudez", LocalDate.of(1986,6, 28),33554109,Gender.MALE, "Lomas", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>345</v>
-      </c>
-      <c r="B26" t="s">
-        <v>346</v>
-      </c>
-      <c r="C26" t="s">
-        <v>278</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>347</v>
-      </c>
-      <c r="F26">
-        <v>31311256</v>
-      </c>
-      <c r="G26" t="s">
-        <v>375</v>
-      </c>
-      <c r="H26" t="s">
-        <v>310</v>
-      </c>
-      <c r="I26" t="s">
-        <v>264</v>
-      </c>
-      <c r="J26" t="s">
-        <v>264</v>
-      </c>
-      <c r="K26" t="s">
-        <v>264</v>
-      </c>
-      <c r="L26" t="s">
-        <v>263</v>
-      </c>
-      <c r="M26" t="s">
-        <v>393</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Anabela", "Lucia", LocalDate.of(1983,8, 12),31311256,Gender.MALE, "Temperley", false, false, false, true, false);</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>326</v>
-      </c>
-      <c r="B27" t="s">
-        <v>348</v>
-      </c>
-      <c r="C27" t="s">
-        <v>303</v>
-      </c>
-      <c r="D27">
-        <v>12</v>
-      </c>
-      <c r="E27" t="s">
-        <v>347</v>
-      </c>
-      <c r="F27">
-        <v>30137911</v>
-      </c>
-      <c r="G27" t="s">
-        <v>375</v>
-      </c>
-      <c r="H27" t="s">
-        <v>292</v>
-      </c>
-      <c r="I27" t="s">
-        <v>263</v>
-      </c>
-      <c r="J27" t="s">
-        <v>264</v>
-      </c>
-      <c r="K27" t="s">
-        <v>264</v>
-      </c>
-      <c r="L27" t="s">
-        <v>264</v>
-      </c>
-      <c r="M27" t="s">
-        <v>393</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Sebastian", "Saccani", LocalDate.of(1985,12, 12),30137911,Gender.MALE, "CABA", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>349</v>
-      </c>
-      <c r="B28" t="s">
-        <v>348</v>
-      </c>
-      <c r="C28" t="s">
-        <v>350</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>351</v>
-      </c>
-      <c r="F28">
-        <v>36009272</v>
-      </c>
-      <c r="G28" t="s">
-        <v>374</v>
-      </c>
-      <c r="H28" t="s">
-        <v>262</v>
-      </c>
-      <c r="I28" t="s">
-        <v>263</v>
-      </c>
-      <c r="J28" t="s">
-        <v>264</v>
-      </c>
-      <c r="K28" t="s">
-        <v>264</v>
-      </c>
-      <c r="L28" t="s">
-        <v>264</v>
-      </c>
-      <c r="M28" t="s">
-        <v>393</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Natalia", "Saccani", LocalDate.of(1989,6, 13),36009272,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>349</v>
-      </c>
-      <c r="B29" t="s">
-        <v>352</v>
-      </c>
-      <c r="C29" t="s">
-        <v>329</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>351</v>
-      </c>
-      <c r="F29">
-        <v>40192827</v>
-      </c>
-      <c r="G29" t="s">
-        <v>375</v>
-      </c>
-      <c r="H29" t="s">
-        <v>262</v>
-      </c>
-      <c r="I29" t="s">
-        <v>264</v>
-      </c>
-      <c r="J29" t="s">
-        <v>264</v>
-      </c>
-      <c r="K29" t="s">
-        <v>264</v>
-      </c>
-      <c r="L29" t="s">
-        <v>263</v>
-      </c>
-      <c r="M29" t="s">
-        <v>393</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Natalia", "Damele", LocalDate.of(1990,1, 13),40192827,Gender.MALE, "Lanus", false, false, false, true, false);</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>353</v>
-      </c>
-      <c r="B30" t="s">
-        <v>354</v>
-      </c>
-      <c r="C30" t="s">
-        <v>355</v>
-      </c>
-      <c r="D30">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>325</v>
-      </c>
-      <c r="F30">
-        <v>45029126</v>
-      </c>
-      <c r="G30" t="s">
-        <v>375</v>
-      </c>
-      <c r="H30" t="s">
-        <v>292</v>
-      </c>
-      <c r="I30" t="s">
-        <v>263</v>
-      </c>
-      <c r="J30" t="s">
-        <v>264</v>
-      </c>
-      <c r="K30" t="s">
-        <v>264</v>
-      </c>
-      <c r="L30" t="s">
-        <v>264</v>
-      </c>
-      <c r="M30" t="s">
-        <v>393</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Eliana", "Matera", LocalDate.of(1994,11, 19),45029126,Gender.MALE, "CABA", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>356</v>
-      </c>
-      <c r="B31" t="s">
-        <v>357</v>
-      </c>
-      <c r="C31" t="s">
-        <v>344</v>
-      </c>
-      <c r="D31">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
-        <v>358</v>
-      </c>
-      <c r="F31">
-        <v>33245927</v>
-      </c>
-      <c r="G31" t="s">
-        <v>374</v>
-      </c>
-      <c r="H31" t="s">
-        <v>283</v>
-      </c>
-      <c r="I31" t="s">
-        <v>263</v>
-      </c>
-      <c r="J31" t="s">
-        <v>264</v>
-      </c>
-      <c r="K31" t="s">
-        <v>264</v>
-      </c>
-      <c r="L31" t="s">
-        <v>264</v>
-      </c>
-      <c r="M31" t="s">
-        <v>393</v>
-      </c>
-      <c r="O31" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Florencia", "Persiani", LocalDate.of(1986,9, 20),33245927,Gender.FEMALE, "Lomas", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>356</v>
-      </c>
-      <c r="B32" t="s">
-        <v>359</v>
-      </c>
-      <c r="C32" t="s">
-        <v>360</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>347</v>
-      </c>
-      <c r="F32">
-        <v>37726189</v>
-      </c>
-      <c r="G32" t="s">
-        <v>374</v>
-      </c>
-      <c r="H32" t="s">
-        <v>262</v>
-      </c>
-      <c r="I32" t="s">
-        <v>264</v>
-      </c>
-      <c r="J32" t="s">
-        <v>264</v>
-      </c>
-      <c r="K32" t="s">
-        <v>264</v>
-      </c>
-      <c r="L32" t="s">
-        <v>263</v>
-      </c>
-      <c r="M32" t="s">
-        <v>393</v>
-      </c>
-      <c r="O32" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Florencia", "De Lucca", LocalDate.of(1991,5, 12),37726189,Gender.FEMALE, "Lanus", false, false, false, true, false);</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>361</v>
-      </c>
-      <c r="B33" t="s">
-        <v>362</v>
-      </c>
-      <c r="C33" t="s">
-        <v>363</v>
-      </c>
-      <c r="D33">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>364</v>
-      </c>
-      <c r="F33">
-        <v>13916645</v>
-      </c>
-      <c r="G33" t="s">
-        <v>375</v>
-      </c>
-      <c r="H33" t="s">
-        <v>292</v>
-      </c>
-      <c r="I33" t="s">
-        <v>263</v>
-      </c>
-      <c r="J33" t="s">
-        <v>264</v>
-      </c>
-      <c r="K33" t="s">
-        <v>264</v>
-      </c>
-      <c r="L33" t="s">
-        <v>264</v>
-      </c>
-      <c r="M33" t="s">
-        <v>393</v>
-      </c>
-      <c r="O33" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Norma", "Ponce", LocalDate.of(1968,5, 4),13916645,Gender.MALE, "CABA", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>356</v>
-      </c>
-      <c r="B34" t="s">
-        <v>365</v>
-      </c>
-      <c r="C34" t="s">
-        <v>366</v>
-      </c>
-      <c r="D34">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>351</v>
-      </c>
-      <c r="F34">
-        <v>46782722</v>
-      </c>
-      <c r="G34" t="s">
-        <v>374</v>
-      </c>
-      <c r="H34" t="s">
-        <v>262</v>
-      </c>
-      <c r="I34" t="s">
-        <v>263</v>
-      </c>
-      <c r="J34" t="s">
-        <v>264</v>
-      </c>
-      <c r="K34" t="s">
-        <v>264</v>
-      </c>
-      <c r="L34" t="s">
-        <v>264</v>
-      </c>
-      <c r="M34" t="s">
-        <v>393</v>
-      </c>
-      <c r="O34" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Florencia", "Salamanca", LocalDate.of(1995,6, 13),46782722,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>367</v>
-      </c>
-      <c r="B35" t="s">
-        <v>368</v>
-      </c>
-      <c r="C35" t="s">
-        <v>286</v>
-      </c>
-      <c r="D35">
-        <v>5</v>
-      </c>
-      <c r="E35" t="s">
-        <v>369</v>
-      </c>
-      <c r="F35">
-        <v>29786687</v>
-      </c>
-      <c r="G35" t="s">
-        <v>374</v>
-      </c>
-      <c r="H35" t="s">
-        <v>262</v>
-      </c>
-      <c r="I35" t="s">
-        <v>263</v>
-      </c>
-      <c r="J35" t="s">
-        <v>264</v>
-      </c>
-      <c r="K35" t="s">
-        <v>264</v>
-      </c>
-      <c r="L35" t="s">
-        <v>264</v>
-      </c>
-      <c r="M35" t="s">
-        <v>393</v>
-      </c>
-      <c r="O35" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Vanesa", "Apodaca", LocalDate.of(1982,5, 14),29786687,Gender.FEMALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>370</v>
-      </c>
-      <c r="B36" t="s">
-        <v>308</v>
-      </c>
-      <c r="C36" t="s">
-        <v>371</v>
-      </c>
-      <c r="D36">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>318</v>
-      </c>
-      <c r="F36">
-        <v>35781115</v>
-      </c>
-      <c r="G36" t="s">
-        <v>375</v>
-      </c>
-      <c r="H36" t="s">
-        <v>262</v>
-      </c>
-      <c r="I36" t="s">
-        <v>263</v>
-      </c>
-      <c r="J36" t="s">
-        <v>264</v>
-      </c>
-      <c r="K36" t="s">
-        <v>264</v>
-      </c>
-      <c r="L36" t="s">
-        <v>264</v>
-      </c>
-      <c r="M36" t="s">
-        <v>393</v>
-      </c>
-      <c r="O36" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Gabriel", "Perez", LocalDate.of(1988,3, 27),35781115,Gender.MALE, "Lanus", true, false, false, false, false);</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>372</v>
-      </c>
-      <c r="B37" t="s">
-        <v>373</v>
-      </c>
-      <c r="C37" t="s">
-        <v>315</v>
-      </c>
-      <c r="D37">
-        <v>7</v>
-      </c>
-      <c r="E37" t="s">
-        <v>296</v>
-      </c>
-      <c r="F37">
-        <v>31766985</v>
-      </c>
-      <c r="G37" t="s">
-        <v>375</v>
-      </c>
-      <c r="H37" t="s">
-        <v>262</v>
-      </c>
-      <c r="I37" t="s">
-        <v>263</v>
-      </c>
-      <c r="J37" t="s">
-        <v>264</v>
-      </c>
-      <c r="K37" t="s">
-        <v>252</v>
-      </c>
-      <c r="L37" t="s">
-        <v>264</v>
-      </c>
-      <c r="M37" t="s">
-        <v>393</v>
-      </c>
-      <c r="O37" t="str">
-        <f t="shared" si="0"/>
-        <v>tempPatient = new Patient("Gonzalo", "Marcec", LocalDate.of(1984,7, 10),31766985,Gender.MALE, "Lanus", true, false,false, false, false);</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37491,15 +37594,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F4D3E87-D9C3-4CF2-AFF5-95DABA850468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBDC475-0F27-4861-89EC-4F8D2CA5B947}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37523,10 +37630,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBDC475-0F27-4861-89EC-4F8D2CA5B947}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F4D3E87-D9C3-4CF2-AFF5-95DABA850468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Caso 8 - Done
</commit_message>
<xml_diff>
--- a/Casos de prueba/Casos de prueba TFI.xlsx
+++ b/Casos de prueba/Casos de prueba TFI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haria\Repositories\TFI-BackEnd\Casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD8BB2F-3C6F-4507-8753-1E31ADD768DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75262A6-8B96-4CD8-B0A4-C87118FD3575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="2" xr2:uid="{E19D2194-C2B1-4B6D-9336-FDF693023F08}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3588" uniqueCount="437">
   <si>
     <t>Operacion</t>
   </si>
@@ -1381,6 +1381,26 @@
   </si>
   <si>
     <t>Se genera el nuevo usuario en el sistema y se solicitan las credenciales para iniciar sesión. Una vez completadas, se recibe el token de acceso.</t>
+  </si>
+  <si>
+    <t>Caso 8</t>
+  </si>
+  <si>
+    <t>Cancelar Turno</t>
+  </si>
+  <si>
+    <t>El usuario cancela uno de sus turnos asignados</t>
+  </si>
+  <si>
+    <t>* El usuario selecciona la opcion "Iniciar Sesión" en el menú principal.
+* Selecciona la opción "Mis turnos".
+* Una vez que se muestran los turnos, presiona el boton de cancdelar turno de uno de los turnos pendientes.</t>
+  </si>
+  <si>
+    <t>Al presionar el botn de cancelar, el usuario volverá a la pantalla de "Mis Turnos" pero el turno se mostrará como "Cancelado".</t>
+  </si>
+  <si>
+    <t>Caso8</t>
   </si>
 </sst>
 </file>
@@ -1838,16 +1858,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1865,16 +1885,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2794,6 +2814,182 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>446</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>505380</xdr:colOff>
+      <xdr:row>486</xdr:row>
+      <xdr:rowOff>30092</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E53777-EB4C-4A37-8982-F7D20CEF3166}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="800100" y="81564480"/>
+          <a:ext cx="10800000" cy="7345292"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>488</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>430080</xdr:colOff>
+      <xdr:row>506</xdr:row>
+      <xdr:rowOff>32522</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14EAFB93-9073-4C89-AD6B-BB519CB800C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792480" y="89245440"/>
+          <a:ext cx="3600000" cy="3324362"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>507</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>497760</xdr:colOff>
+      <xdr:row>546</xdr:row>
+      <xdr:rowOff>101758</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E349B256-838E-43C8-B415-C50FE4366E30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792480" y="92720160"/>
+          <a:ext cx="10800000" cy="7234078"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>548</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>497760</xdr:colOff>
+      <xdr:row>560</xdr:row>
+      <xdr:rowOff>135674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagen 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA3B9A18-3238-4B5B-80D2-29E3AC84E74F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792480" y="100218241"/>
+          <a:ext cx="10800000" cy="2330233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3096,7 +3292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28C3F43-2EA3-4F91-B792-718673B4B8A4}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -14584,10 +14780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DB8F3D-8B49-45A6-A91B-89335D16DD2B}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -14807,7 +15003,7 @@
       </c>
       <c r="D32" s="61"/>
     </row>
-    <row r="33" spans="3:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C33" s="34" t="s">
         <v>224</v>
       </c>
@@ -14815,7 +15011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:4" ht="86.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:4" ht="86.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C34" s="36" t="s">
         <v>429</v>
       </c>
@@ -14823,8 +15019,47 @@
         <v>430</v>
       </c>
     </row>
+    <row r="35" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="36" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A36" t="s">
+        <v>431</v>
+      </c>
+      <c r="C36" s="58" t="s">
+        <v>432</v>
+      </c>
+      <c r="D36" s="59"/>
+    </row>
+    <row r="37" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C37" s="60" t="s">
+        <v>433</v>
+      </c>
+      <c r="D37" s="61"/>
+    </row>
+    <row r="38" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C38" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="72.3" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C39" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>435</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C31:D31"/>
@@ -14834,11 +15069,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14847,10 +15077,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF370F6F-F40A-4D4D-8CDC-9392F0D0A068}">
-  <dimension ref="A1:A332"/>
+  <dimension ref="A1:G489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B429" sqref="B429"/>
+    <sheetView tabSelected="1" topLeftCell="A515" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B549" sqref="B549"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -14888,6 +15118,16 @@
     <row r="332" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>428</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A447" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="489" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G489" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -14943,20 +15183,20 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="74"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
@@ -14985,10 +15225,10 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="72"/>
+      <c r="D11" s="63"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
@@ -15148,7 +15388,7 @@
       <c r="C32" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="D32" s="65"/>
+      <c r="D32" s="74"/>
     </row>
     <row r="33" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C33" s="34" t="s">
@@ -15176,10 +15416,10 @@
       <c r="D36" s="59"/>
     </row>
     <row r="37" spans="3:6" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="71" t="s">
         <v>241</v>
       </c>
-      <c r="D37" s="63"/>
+      <c r="D37" s="72"/>
     </row>
     <row r="38" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C38" s="34" t="s">
@@ -15202,13 +15442,13 @@
       <c r="C41" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="73"/>
     </row>
     <row r="42" spans="3:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C42" s="60" t="s">
         <v>243</v>
       </c>
-      <c r="D42" s="65"/>
+      <c r="D42" s="74"/>
     </row>
     <row r="43" spans="3:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C43" s="34" t="s">
@@ -15228,17 +15468,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C41:D41"/>
@@ -15246,6 +15475,17 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38629,6 +38869,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E4F2C5C2C688D4294DD0A7E4ED187A4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d8ff5051fae7958e87729961111201">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ee180031-54aa-4547-ae85-69ab37712938" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fff74c3b61c94382445f1fd2917e5df0" ns3:_="">
     <xsd:import namespace="ee180031-54aa-4547-ae85-69ab37712938"/>
@@ -38806,12 +39052,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F4D3E87-D9C3-4CF2-AFF5-95DABA850468}">
   <ds:schemaRefs>
@@ -38821,6 +39061,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBDC475-0F27-4861-89EC-4F8D2CA5B947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DE4F7D5-E079-443F-A2F6-B66290943DAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38836,13 +39085,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBDC475-0F27-4861-89EC-4F8D2CA5B947}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>